<commit_message>
Small corrections, cite L. Yao, W. Sethares GA1, GA2
</commit_message>
<xml_diff>
--- a/Project Euler problem 314.xlsx
+++ b/Project Euler problem 314.xlsx
@@ -384,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -458,6 +458,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -6147,7 +6149,7 @@
                   <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>140</c:v>
@@ -6156,13 +6158,13 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>156</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>162</c:v>
@@ -6171,58 +6173,58 @@
                   <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>182</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>190</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>197</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>202</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>208</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>219</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>223</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>228</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>233</c:v>
-                </c:pt>
                 <c:pt idx="26">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>240</c:v>
@@ -6231,13 +6233,13 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>244</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>247</c:v>
@@ -6279,13 +6281,13 @@
                   <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>247</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>246</c:v>
+                  <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>244</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>242</c:v>
@@ -6294,58 +6296,58 @@
                   <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>238</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>237</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>233</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>231</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>228</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>223</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>219</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>214</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>202</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>197</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>185</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>182</c:v>
-                </c:pt>
                 <c:pt idx="26">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>167</c:v>
@@ -6354,13 +6356,13 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>156</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>149</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>145</c:v>
@@ -6369,7 +6371,7 @@
                   <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>134</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>122</c:v>
@@ -6398,7 +6400,7 @@
                   <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>140</c:v>
@@ -6407,13 +6409,13 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>156</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>162</c:v>
@@ -6422,58 +6424,58 @@
                   <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>182</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>190</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>197</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>202</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>208</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>219</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>223</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>228</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>233</c:v>
-                </c:pt>
                 <c:pt idx="26">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>240</c:v>
@@ -6482,13 +6484,13 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>244</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>247</c:v>
@@ -6521,7 +6523,7 @@
                   <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>140</c:v>
@@ -6530,13 +6532,13 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>145</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>156</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>162</c:v>
@@ -6545,58 +6547,58 @@
                   <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>182</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>185</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>190</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>197</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>202</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>208</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>219</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>223</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>228</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>231</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>233</c:v>
-                </c:pt>
                 <c:pt idx="26">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>237</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>238</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>240</c:v>
@@ -6605,13 +6607,13 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>244</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>247</c:v>
@@ -9745,15 +9747,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>326232</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>159545</xdr:rowOff>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>4764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>64294</xdr:rowOff>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -35605,10 +35607,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T101"/>
+  <dimension ref="A1:T106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="G45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q100" sqref="Q100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35701,34 +35703,34 @@
       </c>
       <c r="B3">
         <f ca="1">RAND()/2</f>
-        <v>0.16607121876102321</v>
+        <v>0.30908824489632858</v>
       </c>
       <c r="C3">
         <f ca="1">B3</f>
-        <v>0.16607121876102321</v>
+        <v>0.30908824489632858</v>
       </c>
       <c r="D3">
         <f ca="1">ROUND(52*C3/C$21,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="26">
         <f t="shared" ref="E3:E20" ca="1" si="2">VLOOKUP(D3,xy_lut,2,FALSE)</f>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F3" s="27">
         <v>250</v>
       </c>
       <c r="G3" s="21">
         <f t="shared" ca="1" si="0"/>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H3" s="21">
         <f t="shared" ref="H3" ca="1" si="3">SQRT((E2-E3)^2+(F2-F3)^2)</f>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I3" s="21">
         <f ca="1">E3*F3</f>
-        <v>33250</v>
+        <v>33500</v>
       </c>
       <c r="J3" s="21">
         <v>1</v>
@@ -35774,35 +35776,35 @@
       </c>
       <c r="B4" s="21">
         <f t="shared" ref="B4:B10" ca="1" si="5">RAND()/2</f>
-        <v>1.6729513646813743E-3</v>
+        <v>0.44029041893928267</v>
       </c>
       <c r="C4">
         <f ca="1">C3+B4</f>
-        <v>0.16774417012570458</v>
+        <v>0.74937866383561125</v>
       </c>
       <c r="D4" s="21">
         <f t="shared" ref="D4:D21" ca="1" si="6">ROUND(52*C4/C$21,0)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="F4" s="29">
         <f t="shared" ref="F4:F20" ca="1" si="7">VLOOKUP(D4,xy_lut,3,FALSE)</f>
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G4" s="21">
         <f t="shared" ref="G4:G11" ca="1" si="8">E4</f>
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="H4" s="21">
         <f t="shared" ref="H4:H11" ca="1" si="9">SQRT((E3-E4)^2+(F3-F4)^2)</f>
-        <v>1</v>
+        <v>15.524174696260024</v>
       </c>
       <c r="I4" s="21">
         <f ca="1">(E4-E3)*(F3+F4)/2</f>
-        <v>0</v>
+        <v>3720</v>
       </c>
       <c r="J4" s="21">
         <v>2</v>
@@ -35848,35 +35850,35 @@
       </c>
       <c r="B5" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>1.6947536640842087E-2</v>
+        <v>0.45581356159163583</v>
       </c>
       <c r="C5" s="21">
         <f t="shared" ref="C5:C20" ca="1" si="10">C4+B5</f>
-        <v>0.18469170676654667</v>
+        <v>1.2051922254272471</v>
       </c>
       <c r="D5" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="F5" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="H5" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>1</v>
+        <v>10.440306508910551</v>
       </c>
       <c r="I5" s="21">
         <f t="shared" ref="I5:I39" ca="1" si="11">(E5-E4)*(F4+F5)/2</f>
-        <v>249</v>
+        <v>2445</v>
       </c>
       <c r="J5" s="21">
         <v>3</v>
@@ -35904,7 +35906,7 @@
         <v>6.0827625302982193</v>
       </c>
       <c r="R5" s="21">
-        <f t="shared" ref="R5:R39" si="12">(N5-N4)*(O4+O5)/2</f>
+        <f t="shared" ref="R5:R26" si="12">(N5-N4)*(O4+O5)/2</f>
         <v>1491</v>
       </c>
       <c r="S5" s="21">
@@ -35922,35 +35924,35 @@
       </c>
       <c r="B6" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>5.2202200444905034E-2</v>
+        <v>0.46146626842882171</v>
       </c>
       <c r="C6" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2368939072114517</v>
+        <v>1.6666584938560689</v>
       </c>
       <c r="D6" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="F6" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="H6" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>6.324555320336759</v>
       </c>
       <c r="I6" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>1452</v>
       </c>
       <c r="J6" s="21">
         <v>4</v>
@@ -35996,35 +35998,35 @@
       </c>
       <c r="B7" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.34081868446255892</v>
+        <v>9.181077267052945E-2</v>
       </c>
       <c r="C7" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>0.57771259167401068</v>
+        <v>1.7584692665265984</v>
       </c>
       <c r="D7" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="F7" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="H7" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>15.297058540778355</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="I7" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>3712.5</v>
+        <v>481</v>
       </c>
       <c r="J7" s="21">
         <v>5</v>
@@ -36070,35 +36072,35 @@
       </c>
       <c r="B8" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.42410813462933528</v>
+        <v>6.3730960215531318E-2</v>
       </c>
       <c r="C8" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0018207263033458</v>
+        <v>1.8222002267421298</v>
       </c>
       <c r="D8" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="F8" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G8" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="H8" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>11.401754250991379</v>
+        <v>0</v>
       </c>
       <c r="I8" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>2689.5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="21">
         <v>6</v>
@@ -36144,35 +36146,35 @@
       </c>
       <c r="B9" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>7.8757476841541663E-3</v>
+        <v>0.29481040571233602</v>
       </c>
       <c r="C9" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0096964739875001</v>
+        <v>2.1170106324544657</v>
       </c>
       <c r="D9" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E9" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="F9" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G9" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="I9" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>479</v>
       </c>
       <c r="J9" s="21">
         <v>7</v>
@@ -36218,35 +36220,35 @@
       </c>
       <c r="B10" s="21">
         <f t="shared" ca="1" si="5"/>
-        <v>0.49732423206105664</v>
+        <v>0.41884648923464152</v>
       </c>
       <c r="C10" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.5070207060485568</v>
+        <v>2.5358571216891073</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F10" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G10" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H10" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>8.5440037453175304</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="I10" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>1932</v>
+        <v>1190</v>
       </c>
       <c r="J10" s="21">
         <v>8</v>
@@ -36291,36 +36293,36 @@
         <v>9</v>
       </c>
       <c r="B11" s="21">
-        <f t="shared" ref="B5:B11" ca="1" si="14">RAND()</f>
-        <v>1.4621836188664084E-3</v>
+        <f t="shared" ref="B11" ca="1" si="14">RAND()</f>
+        <v>0.97518565452849881</v>
       </c>
       <c r="C11" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.5084828896674232</v>
+        <v>3.511042776217606</v>
       </c>
       <c r="D11" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="F11" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G11" s="21">
         <f t="shared" ca="1" si="8"/>
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="H11" s="21">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>10.295630140987001</v>
       </c>
       <c r="I11" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>2110.5</v>
       </c>
       <c r="J11" s="21">
         <v>9</v>
@@ -36366,35 +36368,35 @@
       </c>
       <c r="B12" s="21">
         <f t="shared" ref="B4:B21" ca="1" si="15">RAND()</f>
-        <v>0.1719245218982921</v>
+        <v>0.64304799466237839</v>
       </c>
       <c r="C12" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.6804074115657153</v>
+        <v>4.1540907708799839</v>
       </c>
       <c r="D12" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="F12" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="G12" s="21">
         <f t="shared" ref="G12:G20" ca="1" si="16">E12</f>
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="H12" s="21">
         <f ca="1">SQRT((E11-E12)^2+(F11-F12)^2)</f>
-        <v>1.4142135623730951</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="I12" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>239.5</v>
+        <v>1155</v>
       </c>
       <c r="J12" s="21">
         <v>10</v>
@@ -36440,35 +36442,35 @@
       </c>
       <c r="B13" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.61845362159225381</v>
+        <v>0.59640139904687073</v>
       </c>
       <c r="C13" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>2.2988610331579693</v>
+        <v>4.7504921699268543</v>
       </c>
       <c r="D13" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E13" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="F13" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G13" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="H13" s="21">
         <f t="shared" ref="H13:H20" ca="1" si="17">SQRT((E12-E13)^2+(F12-F13)^2)</f>
-        <v>12.083045973594572</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="I13" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>2601.5</v>
+        <v>687</v>
       </c>
       <c r="J13" s="21">
         <v>11</v>
@@ -36514,35 +36516,35 @@
       </c>
       <c r="B14" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.54030598772239691</v>
+        <v>0.66196037954990516</v>
       </c>
       <c r="C14" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>2.8391670208803661</v>
+        <v>5.4124525494767592</v>
       </c>
       <c r="D14" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E14" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="F14" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G14" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>4.4721359549995796</v>
+        <v>6.4031242374328485</v>
       </c>
       <c r="I14" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>932</v>
+        <v>1130</v>
       </c>
       <c r="J14" s="21">
         <v>12</v>
@@ -36588,35 +36590,35 @@
       </c>
       <c r="B15" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.81348410637734636</v>
+        <v>0.16400598863493543</v>
       </c>
       <c r="C15" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>3.6526511272577125</v>
+        <v>5.5764585381116945</v>
       </c>
       <c r="D15" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E15" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="F15" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G15" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>8.0622577482985491</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="I15" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>1610</v>
+        <v>223.5</v>
       </c>
       <c r="J15" s="21">
         <v>13</v>
@@ -36662,35 +36664,35 @@
       </c>
       <c r="B16" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>6.2960191533750542E-2</v>
+        <v>0.67327288509922933</v>
       </c>
       <c r="C16" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>3.715611318791463</v>
+        <v>6.2497314232109238</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E16" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="F16" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G16" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I16" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="J16" s="21">
         <v>14</v>
@@ -36736,35 +36738,35 @@
       </c>
       <c r="B17" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.35377986822085417</v>
+        <v>0.49113456169292824</v>
       </c>
       <c r="C17" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>4.0693911870123172</v>
+        <v>6.7408659849038521</v>
       </c>
       <c r="D17" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="F17" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="H17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>3.6055512754639891</v>
+        <v>2.8284271247461903</v>
       </c>
       <c r="I17" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>678</v>
+        <v>438</v>
       </c>
       <c r="J17" s="21">
         <v>15</v>
@@ -36810,35 +36812,35 @@
       </c>
       <c r="B18" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.86766893475914864</v>
+        <v>2.0874771802830039E-2</v>
       </c>
       <c r="C18" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>4.9370601217714656</v>
+        <v>6.7617407567066818</v>
       </c>
       <c r="D18" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F18" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G18" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>9.4339811320566032</v>
+        <v>0</v>
       </c>
       <c r="I18" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="J18" s="21">
         <v>16</v>
@@ -36884,35 +36886,35 @@
       </c>
       <c r="B19" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.1495151877297668</v>
+        <v>0.28374515648990339</v>
       </c>
       <c r="C19" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>5.0865753095012325</v>
+        <v>7.0454859131965852</v>
       </c>
       <c r="D19" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E19" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F19" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G19" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>217.5</v>
       </c>
       <c r="J19" s="21">
         <v>17</v>
@@ -36958,11 +36960,11 @@
       </c>
       <c r="B20" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.5667195314674851</v>
+        <v>0.17715003503355187</v>
       </c>
       <c r="C20" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>5.6532948409687176</v>
+        <v>7.2226359482301374</v>
       </c>
       <c r="D20" s="21">
         <f t="shared" ca="1" si="6"/>
@@ -36982,11 +36984,11 @@
       </c>
       <c r="H20" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>6.4031242374328485</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>1085</v>
+        <v>648</v>
       </c>
       <c r="J20" s="21">
         <v>18</v>
@@ -37032,11 +37034,11 @@
       </c>
       <c r="B21" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0.43236415498559022</v>
+        <v>0.62534549987887234</v>
       </c>
       <c r="C21" s="21">
         <f t="shared" ref="C21" ca="1" si="19">C20+B21</f>
-        <v>6.0856589959543079</v>
+        <v>7.8479814481090102</v>
       </c>
       <c r="D21" s="21">
         <f t="shared" ca="1" si="6"/>
@@ -37106,23 +37108,23 @@
       </c>
       <c r="E22" s="34">
         <f ca="1">F19</f>
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F22" s="35">
         <f ca="1">E19</f>
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G22" s="21">
         <f t="shared" ref="G22:G39" ca="1" si="22">E22</f>
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H22" s="21">
         <f t="shared" ref="H22:H39" ca="1" si="23">SQRT((E21-E22)^2+(F21-F22)^2)</f>
-        <v>6.4031242374328485</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="I22" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>818</v>
+        <v>411</v>
       </c>
       <c r="J22" s="21">
         <v>20</v>
@@ -37168,23 +37170,23 @@
       </c>
       <c r="E23" s="34">
         <f ca="1">F18</f>
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F23" s="35">
         <f ca="1">E18</f>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G23" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H23" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>1</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="I23" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>202</v>
+        <v>203.5</v>
       </c>
       <c r="J23" s="21">
         <v>21</v>
@@ -37230,23 +37232,23 @@
       </c>
       <c r="E24" s="34">
         <f ca="1">F17</f>
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F24" s="35">
         <f ca="1">E17</f>
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="G24" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H24" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>9.4339811320566032</v>
+        <v>0</v>
       </c>
       <c r="I24" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>990</v>
+        <v>0</v>
       </c>
       <c r="J24" s="21">
         <v>22</v>
@@ -37292,23 +37294,23 @@
       </c>
       <c r="E25" s="34">
         <f ca="1">F16</f>
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F25" s="35">
         <f ca="1">E16</f>
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="G25" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H25" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>3.6055512754639891</v>
+        <v>2.8284271247461903</v>
       </c>
       <c r="I25" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>385</v>
+        <v>404</v>
       </c>
       <c r="J25" s="21">
         <v>23</v>
@@ -37354,23 +37356,23 @@
       </c>
       <c r="E26" s="34">
         <f ca="1">F15</f>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F26" s="35">
         <f ca="1">E15</f>
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="G26" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H26" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I26" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>191</v>
+        <v>597</v>
       </c>
       <c r="J26" s="21">
         <v>24</v>
@@ -37416,23 +37418,23 @@
       </c>
       <c r="E27" s="34">
         <f ca="1">F14</f>
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F27" s="35">
         <f ca="1">E14</f>
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="G27" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H27" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>8.0622577482985491</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="I27" s="21">
         <f ca="1">(E27-E26)*(F26+F27)/2</f>
-        <v>750</v>
+        <v>196.5</v>
       </c>
       <c r="J27" s="21">
         <v>25</v>
@@ -37478,23 +37480,23 @@
       </c>
       <c r="E28" s="34">
         <f ca="1">F13</f>
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F28" s="35">
         <f ca="1">E13</f>
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="G28" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H28" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>4.4721359549995796</v>
+        <v>6.4031242374328485</v>
       </c>
       <c r="I28" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>364</v>
+        <v>774</v>
       </c>
       <c r="J28" s="21">
         <v>26</v>
@@ -37522,7 +37524,7 @@
         <v>3.6055512754639891</v>
       </c>
       <c r="R28" s="21">
-        <f t="shared" ref="R28:R41" si="24">(N28-N27)*(O27+O28)/2</f>
+        <f t="shared" ref="R28:R39" si="24">(N28-N27)*(O27+O28)/2</f>
         <v>373</v>
       </c>
       <c r="S28" s="21">
@@ -37540,23 +37542,23 @@
       </c>
       <c r="E29" s="34">
         <f ca="1">F12</f>
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F29" s="35">
         <f ca="1">E12</f>
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="G29" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="H29" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>12.083045973594572</v>
+        <v>3.6055512754639891</v>
       </c>
       <c r="I29" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>872.5</v>
+        <v>379</v>
       </c>
       <c r="J29" s="21">
         <v>27</v>
@@ -37602,23 +37604,23 @@
       </c>
       <c r="E30" s="34">
         <f ca="1">F11</f>
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F30" s="35">
         <f ca="1">E11</f>
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="G30" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H30" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>1.4142135623730951</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="I30" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>168.5</v>
+        <v>371</v>
       </c>
       <c r="J30" s="21">
         <v>28</v>
@@ -37664,23 +37666,23 @@
       </c>
       <c r="E31" s="34">
         <f ca="1">F10</f>
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F31" s="35">
         <f ca="1">E10</f>
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G31" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H31" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>0</v>
+        <v>10.295630140987001</v>
       </c>
       <c r="I31" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>892.5</v>
       </c>
       <c r="J31" s="21">
         <v>29</v>
@@ -37726,23 +37728,23 @@
       </c>
       <c r="E32" s="34">
         <f ca="1">F9</f>
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F32" s="35">
         <f ca="1">E9</f>
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="G32" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H32" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>8.5440037453175304</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="I32" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>492</v>
+        <v>343</v>
       </c>
       <c r="J32" s="21">
         <v>30</v>
@@ -37788,23 +37790,23 @@
       </c>
       <c r="E33" s="34">
         <f ca="1">F8</f>
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F33" s="35">
         <f ca="1">E8</f>
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="G33" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H33" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>0</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="I33" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="J33" s="21">
         <v>31</v>
@@ -37850,23 +37852,23 @@
       </c>
       <c r="E34" s="34">
         <f ca="1">F7</f>
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F34" s="35">
         <f ca="1">E7</f>
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G34" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H34" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>11.401754250991379</v>
+        <v>0</v>
       </c>
       <c r="I34" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>463.5</v>
+        <v>0</v>
       </c>
       <c r="J34" s="21">
         <v>32</v>
@@ -37912,23 +37914,23 @@
       </c>
       <c r="E35" s="34">
         <f ca="1">F6</f>
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F35" s="35">
         <f ca="1">E6</f>
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="G35" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="H35" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>15.297058540778355</v>
+        <v>2.2360679774997898</v>
       </c>
       <c r="I35" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>424.5</v>
+        <v>166</v>
       </c>
       <c r="J35" s="21">
         <v>33</v>
@@ -37974,23 +37976,23 @@
       </c>
       <c r="E36" s="34">
         <f ca="1">F5</f>
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="F36" s="35">
         <f ca="1">E5</f>
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="G36" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="H36" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>0</v>
+        <v>6.324555320336759</v>
       </c>
       <c r="I36" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>324</v>
       </c>
       <c r="J36" s="21">
         <v>34</v>
@@ -38036,23 +38038,23 @@
       </c>
       <c r="E37" s="34">
         <f ca="1">F4</f>
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F37" s="35">
         <f ca="1">E4</f>
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="G37" s="21">
         <f t="shared" ca="1" si="22"/>
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H37" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>1</v>
+        <v>10.440306508910551</v>
       </c>
       <c r="I37" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>0</v>
+        <v>462</v>
       </c>
       <c r="J37" s="21">
         <v>35</v>
@@ -38102,7 +38104,7 @@
       </c>
       <c r="F38" s="35">
         <f ca="1">E3</f>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G38" s="21">
         <f t="shared" si="22"/>
@@ -38110,11 +38112,11 @@
       </c>
       <c r="H38" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>1</v>
+        <v>15.524174696260024</v>
       </c>
       <c r="I38" s="21">
         <f t="shared" ca="1" si="11"/>
-        <v>133</v>
+        <v>566</v>
       </c>
       <c r="J38" s="21">
         <v>36</v>
@@ -38172,7 +38174,7 @@
       </c>
       <c r="H39" s="21">
         <f t="shared" ca="1" si="23"/>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I39" s="21">
         <f t="shared" ca="1" si="11"/>
@@ -38220,15 +38222,15 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G41" s="4">
         <f ca="1">I41/H41</f>
-        <v>131.39623474434913</v>
+        <v>132.37127037442377</v>
       </c>
       <c r="H41" s="21">
         <f ca="1">SUM(H3:H39)</f>
-        <v>446.74796134159783</v>
+        <v>443.5101350462171</v>
       </c>
       <c r="I41" s="21">
         <f ca="1">SUM(I3:I39)</f>
-        <v>58701</v>
+        <v>58708</v>
       </c>
       <c r="P41" s="4">
         <f>R41/Q41</f>
@@ -38306,7 +38308,8 @@
         <f t="shared" ref="E47:E97" si="26">"{"&amp;B47&amp;", "&amp;C47&amp;"}, "</f>
         <v xml:space="preserve">{133, 249}, </v>
       </c>
-      <c r="G47" s="21">
+      <c r="G47" s="23">
+        <f>Q87</f>
         <v>0</v>
       </c>
       <c r="H47" s="38">
@@ -38314,7 +38317,6 @@
         <v>122</v>
       </c>
       <c r="I47" s="38">
-        <f>VLOOKUP(G47,xy_lut,3,FALSE)</f>
         <v>250</v>
       </c>
       <c r="J47" s="21">
@@ -38345,12 +38347,13 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{134, 249}, </v>
       </c>
-      <c r="G48" s="21">
-        <v>2</v>
+      <c r="G48" s="23">
+        <f t="shared" ref="G48:G64" si="28">Q88</f>
+        <v>1</v>
       </c>
       <c r="H48" s="38">
         <f>VLOOKUP(G48,xy_lut,2,FALSE)</f>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I48" s="38">
         <f>VLOOKUP(G48,xy_lut,3,FALSE)</f>
@@ -38358,15 +38361,15 @@
       </c>
       <c r="J48" s="21">
         <f t="shared" si="25"/>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K48" s="21">
         <f t="shared" si="27"/>
-        <v>12.041594578792296</v>
+        <v>11.045361017187261</v>
       </c>
       <c r="L48" s="21">
         <f>(H48-H47)*(I47+I48)/2</f>
-        <v>2994</v>
+        <v>2744.5</v>
       </c>
       <c r="O48" s="21"/>
     </row>
@@ -38384,7 +38387,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{140, 248}, </v>
       </c>
-      <c r="G49" s="21">
+      <c r="G49" s="23">
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="H49" s="38">
@@ -38401,11 +38405,11 @@
       </c>
       <c r="K49" s="21">
         <f t="shared" si="27"/>
-        <v>6.0827625302982193</v>
+        <v>7.0710678118654755</v>
       </c>
       <c r="L49" s="21">
-        <f t="shared" ref="L49:L83" si="28">(H49-H48)*(I48+I49)/2</f>
-        <v>1491</v>
+        <f t="shared" ref="L49:L70" si="29">(H49-H48)*(I48+I49)/2</f>
+        <v>1739.5</v>
       </c>
       <c r="O49" s="21"/>
     </row>
@@ -38423,7 +38427,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{145, 247}, </v>
       </c>
-      <c r="G50" s="21">
+      <c r="G50" s="23">
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="H50" s="38">
@@ -38443,7 +38448,7 @@
         <v>5.0990195135927845</v>
       </c>
       <c r="L50" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1237.5</v>
       </c>
       <c r="O50" s="21"/>
@@ -38462,28 +38467,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{149, 246}, </v>
       </c>
-      <c r="G51" s="21">
-        <v>4</v>
+      <c r="G51" s="23">
+        <f t="shared" si="28"/>
+        <v>5</v>
       </c>
       <c r="H51" s="38">
         <f>VLOOKUP(G51,xy_lut,2,FALSE)</f>
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="I51" s="38">
         <f>VLOOKUP(G51,xy_lut,3,FALSE)</f>
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J51" s="21">
         <f t="shared" si="25"/>
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="K51" s="21">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>4.1231056256176606</v>
       </c>
       <c r="L51" s="21">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>986</v>
       </c>
       <c r="O51" s="21"/>
     </row>
@@ -38501,28 +38507,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{153, 245}, </v>
       </c>
-      <c r="G52" s="21">
-        <v>5</v>
+      <c r="G52" s="23">
+        <f t="shared" si="28"/>
+        <v>7</v>
       </c>
       <c r="H52" s="38">
         <f>VLOOKUP(G52,xy_lut,2,FALSE)</f>
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="I52" s="38">
         <f>VLOOKUP(G52,xy_lut,3,FALSE)</f>
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J52" s="21">
         <f t="shared" si="25"/>
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="K52" s="21">
         <f t="shared" si="27"/>
-        <v>4.1231056256176606</v>
+        <v>7.2801098892805181</v>
       </c>
       <c r="L52" s="21">
-        <f t="shared" si="28"/>
-        <v>986</v>
+        <f t="shared" si="29"/>
+        <v>1715</v>
       </c>
       <c r="O52" s="21"/>
     </row>
@@ -38540,28 +38547,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{156, 244}, </v>
       </c>
-      <c r="G53" s="21">
-        <v>7</v>
+      <c r="G53" s="23">
+        <f t="shared" si="28"/>
+        <v>10</v>
       </c>
       <c r="H53" s="38">
         <f>VLOOKUP(G53,xy_lut,2,FALSE)</f>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="I53" s="38">
         <f>VLOOKUP(G53,xy_lut,3,FALSE)</f>
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J53" s="21">
         <f t="shared" si="25"/>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K53" s="21">
         <f t="shared" si="27"/>
-        <v>7.2801098892805181</v>
+        <v>6.324555320336759</v>
       </c>
       <c r="L53" s="21">
-        <f t="shared" si="28"/>
-        <v>1715</v>
+        <f t="shared" si="29"/>
+        <v>1458</v>
       </c>
       <c r="O53" s="21"/>
     </row>
@@ -38579,7 +38587,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{159, 243}, </v>
       </c>
-      <c r="G54" s="21">
+      <c r="G54" s="23">
+        <f t="shared" si="28"/>
         <v>10</v>
       </c>
       <c r="H54" s="38">
@@ -38596,11 +38605,11 @@
       </c>
       <c r="K54" s="21">
         <f t="shared" si="27"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
       <c r="L54" s="21">
-        <f t="shared" si="28"/>
-        <v>1458</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
       </c>
       <c r="O54" s="21"/>
     </row>
@@ -38618,7 +38627,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{160, 243}, </v>
       </c>
-      <c r="G55" s="21">
+      <c r="G55" s="23">
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="H55" s="38">
@@ -38638,7 +38648,7 @@
         <v>5.3851648071345037</v>
       </c>
       <c r="L55" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1205</v>
       </c>
       <c r="O55" s="21"/>
@@ -38657,28 +38667,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{162, 242}, </v>
       </c>
-      <c r="G56" s="21">
-        <v>16</v>
+      <c r="G56" s="23">
+        <f t="shared" si="28"/>
+        <v>17</v>
       </c>
       <c r="H56" s="38">
         <f>VLOOKUP(G56,xy_lut,2,FALSE)</f>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I56" s="38">
         <f>VLOOKUP(G56,xy_lut,3,FALSE)</f>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J56" s="21">
         <f t="shared" si="25"/>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="K56" s="21">
         <f>SQRT((H55-H56)^2+(I55-I56)^2)</f>
-        <v>5.3851648071345037</v>
+        <v>7.6157731058639087</v>
       </c>
       <c r="L56" s="21">
-        <f t="shared" si="28"/>
-        <v>1195</v>
+        <f t="shared" si="29"/>
+        <v>1669.5</v>
       </c>
       <c r="O56" s="21"/>
     </row>
@@ -38696,28 +38707,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{165, 241}, </v>
       </c>
-      <c r="G57" s="21">
-        <v>17</v>
+      <c r="G57" s="23">
+        <f t="shared" si="28"/>
+        <v>19</v>
       </c>
       <c r="H57" s="38">
         <f>VLOOKUP(G57,xy_lut,2,FALSE)</f>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I57" s="38">
         <f>VLOOKUP(G57,xy_lut,3,FALSE)</f>
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J57" s="21">
         <f t="shared" si="25"/>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="K57" s="21">
-        <f t="shared" ref="K57:K83" si="29">SQRT((H56-H57)^2+(I56-I57)^2)</f>
-        <v>2.2360679774997898</v>
+        <f t="shared" ref="K57:K83" si="30">SQRT((H56-H57)^2+(I56-I57)^2)</f>
+        <v>4.4721359549995796</v>
       </c>
       <c r="L57" s="21">
-        <f t="shared" si="28"/>
-        <v>475</v>
+        <f t="shared" si="29"/>
+        <v>944</v>
       </c>
       <c r="O57" s="21"/>
     </row>
@@ -38735,28 +38747,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{167, 240}, </v>
       </c>
-      <c r="G58" s="21">
-        <v>21</v>
+      <c r="G58" s="23">
+        <f t="shared" si="28"/>
+        <v>26</v>
       </c>
       <c r="H58" s="38">
         <f>VLOOKUP(G58,xy_lut,2,FALSE)</f>
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I58" s="38">
         <f>VLOOKUP(G58,xy_lut,3,FALSE)</f>
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J58" s="21">
         <f t="shared" si="25"/>
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="K58" s="21">
+        <f t="shared" si="30"/>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="L58" s="21">
         <f t="shared" si="29"/>
-        <v>8.9442719099991592</v>
-      </c>
-      <c r="L58" s="21">
-        <f t="shared" si="28"/>
-        <v>1880</v>
+        <v>1631</v>
       </c>
       <c r="O58" s="21"/>
     </row>
@@ -38774,28 +38787,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{168, 240}, </v>
       </c>
-      <c r="G59" s="21">
-        <v>26</v>
+      <c r="G59" s="23">
+        <f t="shared" si="28"/>
+        <v>30</v>
       </c>
       <c r="H59" s="38">
         <f>VLOOKUP(G59,xy_lut,2,FALSE)</f>
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="I59" s="38">
         <f>VLOOKUP(G59,xy_lut,3,FALSE)</f>
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J59" s="21">
         <f t="shared" si="25"/>
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="K59" s="21">
+        <f t="shared" si="30"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="L59" s="21">
         <f t="shared" si="29"/>
-        <v>3.6055512754639891</v>
-      </c>
-      <c r="L59" s="21">
-        <f t="shared" si="28"/>
-        <v>696</v>
+        <v>1147.5</v>
       </c>
       <c r="O59" s="21"/>
     </row>
@@ -38813,28 +38827,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{169, 239}, </v>
       </c>
-      <c r="G60">
-        <v>30</v>
+      <c r="G60" s="23">
+        <f t="shared" si="28"/>
+        <v>33</v>
       </c>
       <c r="H60" s="38">
         <f>VLOOKUP(G60,xy_lut,2,FALSE)</f>
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I60" s="38">
         <f>VLOOKUP(G60,xy_lut,3,FALSE)</f>
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J60" s="21">
         <f t="shared" si="25"/>
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="K60" s="21">
+        <f t="shared" si="30"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="L60" s="21">
         <f t="shared" si="29"/>
-        <v>5.8309518948453007</v>
-      </c>
-      <c r="L60" s="21">
-        <f t="shared" si="28"/>
-        <v>1147.5</v>
+        <v>681</v>
       </c>
       <c r="O60" s="21"/>
     </row>
@@ -38852,7 +38867,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{170, 239}, </v>
       </c>
-      <c r="G61">
+      <c r="G61" s="23">
+        <f t="shared" si="28"/>
         <v>33</v>
       </c>
       <c r="H61" s="38">
@@ -38868,12 +38884,12 @@
         <v>193</v>
       </c>
       <c r="K61" s="21">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="L61" s="21">
         <f t="shared" si="29"/>
-        <v>3.6055512754639891</v>
-      </c>
-      <c r="L61" s="21">
-        <f t="shared" si="28"/>
-        <v>681</v>
+        <v>0</v>
       </c>
       <c r="O61" s="21"/>
     </row>
@@ -38891,28 +38907,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{172, 238}, </v>
       </c>
-      <c r="G62" s="21">
-        <v>37</v>
+      <c r="G62" s="23">
+        <f t="shared" si="28"/>
+        <v>41</v>
       </c>
       <c r="H62" s="38">
         <f>VLOOKUP(G62,xy_lut,2,FALSE)</f>
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="I62" s="38">
         <f>VLOOKUP(G62,xy_lut,3,FALSE)</f>
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J62" s="21">
         <f t="shared" si="25"/>
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K62" s="21">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="L62" s="21">
         <f t="shared" si="29"/>
-        <v>5</v>
-      </c>
-      <c r="L62" s="21">
-        <f t="shared" si="28"/>
-        <v>898</v>
+        <v>1784</v>
       </c>
       <c r="O62" s="21"/>
     </row>
@@ -38930,28 +38947,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{174, 237}, </v>
       </c>
-      <c r="G63" s="21">
-        <v>43</v>
+      <c r="G63" s="23">
+        <f t="shared" si="28"/>
+        <v>49</v>
       </c>
       <c r="H63" s="38">
         <f>VLOOKUP(G63,xy_lut,2,FALSE)</f>
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="I63" s="38">
         <f>VLOOKUP(G63,xy_lut,3,FALSE)</f>
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="J63" s="21">
         <f t="shared" si="25"/>
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="K63" s="21">
+        <f t="shared" si="30"/>
+        <v>9.2195444572928871</v>
+      </c>
+      <c r="L63" s="21">
         <f t="shared" si="29"/>
-        <v>6.4031242374328485</v>
-      </c>
-      <c r="L63" s="21">
-        <f t="shared" si="28"/>
-        <v>1105</v>
+        <v>1519</v>
       </c>
       <c r="O63" s="21"/>
     </row>
@@ -38969,28 +38987,29 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{176, 236}, </v>
       </c>
-      <c r="G64" s="21">
-        <v>49</v>
+      <c r="G64" s="23">
+        <f t="shared" si="28"/>
+        <v>50</v>
       </c>
       <c r="H64" s="38">
         <f>VLOOKUP(G64,xy_lut,2,FALSE)</f>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I64" s="38">
         <f>VLOOKUP(G64,xy_lut,3,FALSE)</f>
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J64" s="21">
         <f t="shared" si="25"/>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K64" s="21">
+        <f t="shared" si="30"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="L64" s="21">
         <f t="shared" si="29"/>
-        <v>7.810249675906654</v>
-      </c>
-      <c r="L64" s="21">
-        <f t="shared" si="28"/>
-        <v>1299</v>
+        <v>213.5</v>
       </c>
       <c r="O64" s="21"/>
     </row>
@@ -39011,23 +39030,23 @@
       <c r="G65" s="21"/>
       <c r="H65" s="32">
         <f>I64</f>
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I65" s="33">
         <f>H64</f>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J65" s="21">
         <f t="shared" si="25"/>
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K65" s="21">
+        <f t="shared" si="30"/>
+        <v>5.6568542494923806</v>
+      </c>
+      <c r="L65" s="21">
         <f t="shared" si="29"/>
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="L65" s="21">
-        <f t="shared" si="28"/>
-        <v>1266</v>
+        <v>844</v>
       </c>
       <c r="O65" s="21"/>
     </row>
@@ -39048,23 +39067,23 @@
       <c r="G66" s="21"/>
       <c r="H66" s="34">
         <f>I63</f>
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I66" s="35">
         <f>H63</f>
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J66" s="21">
         <f t="shared" si="25"/>
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="K66" s="21">
+        <f t="shared" si="30"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="L66" s="21">
         <f t="shared" si="29"/>
-        <v>7.810249675906654</v>
-      </c>
-      <c r="L66" s="21">
-        <f t="shared" si="28"/>
-        <v>1025</v>
+        <v>208.5</v>
       </c>
       <c r="O66" s="21"/>
     </row>
@@ -39085,23 +39104,23 @@
       <c r="G67" s="21"/>
       <c r="H67" s="34">
         <f>I62</f>
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I67" s="35">
         <f>H62</f>
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="J67" s="21">
         <f t="shared" si="25"/>
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K67" s="21">
+        <f t="shared" si="30"/>
+        <v>9.2195444572928871</v>
+      </c>
+      <c r="L67" s="21">
         <f t="shared" si="29"/>
-        <v>6.4031242374328485</v>
-      </c>
-      <c r="L67" s="21">
-        <f t="shared" si="28"/>
-        <v>798</v>
+        <v>1227</v>
       </c>
       <c r="O67" s="21"/>
     </row>
@@ -39133,12 +39152,12 @@
         <v>226</v>
       </c>
       <c r="K68" s="21">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="L68" s="21">
         <f t="shared" si="29"/>
-        <v>5</v>
-      </c>
-      <c r="L68" s="21">
-        <f t="shared" si="28"/>
-        <v>585</v>
+        <v>1182</v>
       </c>
       <c r="O68" s="21"/>
     </row>
@@ -39159,23 +39178,23 @@
       <c r="G69" s="21"/>
       <c r="H69" s="34">
         <f>I60</f>
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I69" s="35">
         <f>H60</f>
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J69" s="21">
         <f t="shared" si="25"/>
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K69" s="21">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="21">
         <f t="shared" si="29"/>
-        <v>3.6055512754639891</v>
-      </c>
-      <c r="L69" s="21">
-        <f t="shared" si="28"/>
-        <v>383</v>
+        <v>0</v>
       </c>
       <c r="O69" s="21"/>
     </row>
@@ -39196,23 +39215,23 @@
       <c r="G70" s="21"/>
       <c r="H70" s="34">
         <f>I59</f>
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="I70" s="35">
         <f>H59</f>
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="J70" s="21">
         <f t="shared" si="25"/>
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="K70" s="21">
+        <f t="shared" si="30"/>
+        <v>3.6055512754639891</v>
+      </c>
+      <c r="L70" s="21">
         <f t="shared" si="29"/>
-        <v>5.8309518948453007</v>
-      </c>
-      <c r="L70" s="21">
-        <f t="shared" si="28"/>
-        <v>562.5</v>
+        <v>383</v>
       </c>
       <c r="O70" s="21"/>
     </row>
@@ -39233,23 +39252,23 @@
       <c r="G71" s="21"/>
       <c r="H71" s="34">
         <f>I58</f>
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I71" s="35">
         <f>H58</f>
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="J71" s="21">
         <f t="shared" si="25"/>
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K71" s="21">
-        <f t="shared" si="29"/>
-        <v>3.6055512754639891</v>
+        <f t="shared" si="30"/>
+        <v>5.8309518948453007</v>
       </c>
       <c r="L71" s="21">
         <f>(H71-H70)*(I70+I71)/2</f>
-        <v>367</v>
+        <v>562.5</v>
       </c>
       <c r="O71" s="21"/>
     </row>
@@ -39270,23 +39289,23 @@
       <c r="G72" s="21"/>
       <c r="H72" s="34">
         <f>I57</f>
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I72" s="35">
         <f>H57</f>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="J72" s="21">
         <f t="shared" si="25"/>
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K72" s="21">
-        <f t="shared" si="29"/>
-        <v>8.9442719099991592</v>
+        <f t="shared" si="30"/>
+        <v>8.0622577482985491</v>
       </c>
       <c r="L72" s="21">
-        <f t="shared" ref="L72:L85" si="30">(H72-H71)*(I71+I72)/2</f>
-        <v>712</v>
+        <f t="shared" ref="L72:L83" si="31">(H72-H71)*(I71+I72)/2</f>
+        <v>726</v>
       </c>
       <c r="O72" s="21"/>
     </row>
@@ -39307,23 +39326,23 @@
       <c r="G73" s="21"/>
       <c r="H73" s="34">
         <f>I56</f>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I73" s="35">
         <f>H56</f>
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="J73" s="21">
         <f t="shared" si="25"/>
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K73" s="21">
-        <f t="shared" si="29"/>
-        <v>2.2360679774997898</v>
+        <f t="shared" si="30"/>
+        <v>4.4721359549995796</v>
       </c>
       <c r="L73" s="21">
-        <f t="shared" si="30"/>
-        <v>173</v>
+        <f t="shared" si="31"/>
+        <v>352</v>
       </c>
       <c r="O73" s="21"/>
     </row>
@@ -39355,12 +39374,12 @@
         <v>240</v>
       </c>
       <c r="K74" s="21">
-        <f t="shared" si="29"/>
-        <v>5.3851648071345037</v>
+        <f t="shared" si="30"/>
+        <v>7.6157731058639087</v>
       </c>
       <c r="L74" s="21">
-        <f t="shared" si="30"/>
-        <v>339</v>
+        <f t="shared" si="31"/>
+        <v>511.5</v>
       </c>
       <c r="O74" s="21"/>
     </row>
@@ -39392,11 +39411,11 @@
         <v>242</v>
       </c>
       <c r="K75" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>5.3851648071345037</v>
       </c>
       <c r="L75" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>329</v>
       </c>
       <c r="O75" s="21"/>
@@ -39418,23 +39437,23 @@
       <c r="G76" s="21"/>
       <c r="H76" s="34">
         <f>I53</f>
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I76" s="35">
         <f>H53</f>
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="J76" s="21">
         <f t="shared" si="25"/>
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="K76" s="21">
-        <f t="shared" si="29"/>
-        <v>6.324555320336759</v>
+        <f t="shared" si="30"/>
+        <v>0</v>
       </c>
       <c r="L76" s="21">
-        <f t="shared" si="30"/>
-        <v>318</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="O76" s="21"/>
     </row>
@@ -39455,23 +39474,23 @@
       <c r="G77" s="21"/>
       <c r="H77" s="34">
         <f>I52</f>
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I77" s="35">
         <f>H52</f>
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="J77" s="21">
         <f t="shared" si="25"/>
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K77" s="21">
-        <f t="shared" si="29"/>
-        <v>7.2801098892805181</v>
+        <f t="shared" si="30"/>
+        <v>6.324555320336759</v>
       </c>
       <c r="L77" s="21">
-        <f t="shared" si="30"/>
-        <v>305</v>
+        <f t="shared" si="31"/>
+        <v>318</v>
       </c>
       <c r="O77" s="21"/>
     </row>
@@ -39492,23 +39511,23 @@
       <c r="G78" s="21"/>
       <c r="H78" s="34">
         <f>I51</f>
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I78" s="35">
         <f>H51</f>
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="J78" s="21">
         <f t="shared" si="25"/>
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K78" s="21">
-        <f t="shared" si="29"/>
-        <v>4.1231056256176606</v>
+        <f t="shared" si="30"/>
+        <v>7.2801098892805181</v>
       </c>
       <c r="L78" s="21">
-        <f t="shared" si="30"/>
-        <v>147</v>
+        <f t="shared" si="31"/>
+        <v>305</v>
       </c>
       <c r="O78" s="21"/>
     </row>
@@ -39540,12 +39559,12 @@
         <v>247</v>
       </c>
       <c r="K79" s="21">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <f t="shared" si="30"/>
+        <v>4.1231056256176606</v>
       </c>
       <c r="L79" s="21">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>147</v>
       </c>
       <c r="O79" s="21"/>
     </row>
@@ -39577,16 +39596,16 @@
         <v>248</v>
       </c>
       <c r="K80" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>5.0990195135927845</v>
       </c>
       <c r="L80" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>142.5</v>
       </c>
       <c r="O80" s="21"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="21">
         <v>35</v>
       </c>
@@ -39607,23 +39626,23 @@
       </c>
       <c r="I81" s="35">
         <f>H48</f>
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J81" s="21">
         <f t="shared" si="25"/>
         <v>249</v>
       </c>
       <c r="K81" s="21">
-        <f t="shared" si="29"/>
-        <v>6.0827625302982193</v>
+        <f t="shared" si="30"/>
+        <v>7.0710678118654755</v>
       </c>
       <c r="L81" s="21">
-        <f t="shared" si="30"/>
-        <v>137</v>
+        <f t="shared" si="31"/>
+        <v>136.5</v>
       </c>
       <c r="O81" s="21"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="21">
         <v>36</v>
       </c>
@@ -39651,15 +39670,15 @@
         <v>250</v>
       </c>
       <c r="K82" s="21">
-        <f t="shared" si="29"/>
-        <v>12.041594578792296</v>
+        <f t="shared" si="30"/>
+        <v>11.045361017187261</v>
       </c>
       <c r="L82" s="21">
-        <f t="shared" si="30"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="31"/>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="21">
         <v>37</v>
       </c>
@@ -39687,15 +39706,15 @@
         <v>250</v>
       </c>
       <c r="K83" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>122</v>
       </c>
       <c r="L83" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="21">
         <v>38</v>
       </c>
@@ -39709,14 +39728,10 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{198, 223}, </v>
       </c>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
-      <c r="J84" s="21"/>
       <c r="K84" s="21"/>
       <c r="L84" s="21"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="21">
         <v>39</v>
       </c>
@@ -39730,22 +39745,20 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{198, 222}, </v>
       </c>
-      <c r="H85" s="21"/>
-      <c r="I85" s="21"/>
       <c r="K85" s="21">
         <f>SUM(K47:K83)</f>
-        <v>442.79977201183658</v>
+        <v>442.75447821779704</v>
       </c>
       <c r="L85" s="21">
         <f>SUM(L47:L83)</f>
-        <v>58680</v>
+        <v>58677</v>
       </c>
       <c r="M85" s="4">
         <f>L85/K85</f>
-        <v>132.52039343514252</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+        <v>132.52717451032979</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="21">
         <v>40</v>
       </c>
@@ -39759,11 +39772,8 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{200, 221}, </v>
       </c>
-      <c r="G86" s="21"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="21">
         <v>41</v>
       </c>
@@ -39777,11 +39787,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{201, 220}, </v>
       </c>
-      <c r="G87" s="21"/>
+      <c r="G87" s="21">
+        <v>0</v>
+      </c>
       <c r="H87" s="21"/>
-      <c r="I87" s="21"/>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I87" s="21">
+        <v>0</v>
+      </c>
+      <c r="J87" s="21">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q87" s="23">
+        <v>0</v>
+      </c>
+      <c r="R87" s="21"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="21">
         <v>42</v>
       </c>
@@ -39795,11 +39831,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{202, 220}, </v>
       </c>
-      <c r="G88" s="21"/>
+      <c r="G88" s="21">
+        <v>2</v>
+      </c>
       <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I88" s="21">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>2</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>1</v>
+      </c>
+      <c r="N88">
+        <v>1</v>
+      </c>
+      <c r="O88" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="23">
+        <v>1</v>
+      </c>
+      <c r="R88" s="21"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="21">
         <v>43</v>
       </c>
@@ -39813,11 +39875,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{202, 219}, </v>
       </c>
-      <c r="G89" s="21"/>
+      <c r="G89" s="21">
+        <v>3</v>
+      </c>
       <c r="H89" s="21"/>
-      <c r="I89" s="21"/>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I89" s="21">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>3</v>
+      </c>
+      <c r="K89">
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <v>2</v>
+      </c>
+      <c r="M89">
+        <v>3</v>
+      </c>
+      <c r="N89">
+        <v>3</v>
+      </c>
+      <c r="O89" s="23">
+        <v>3</v>
+      </c>
+      <c r="Q89" s="23">
+        <v>3</v>
+      </c>
+      <c r="R89" s="21"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="21">
         <v>44</v>
       </c>
@@ -39831,11 +39919,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{203, 219}, </v>
       </c>
-      <c r="G90" s="21"/>
+      <c r="G90" s="21">
+        <v>4</v>
+      </c>
       <c r="H90" s="21"/>
-      <c r="I90" s="21"/>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I90" s="39">
+        <v>3</v>
+      </c>
+      <c r="J90" s="39">
+        <v>4</v>
+      </c>
+      <c r="K90" s="39">
+        <v>4</v>
+      </c>
+      <c r="L90" s="39">
+        <v>3</v>
+      </c>
+      <c r="M90" s="39">
+        <v>3</v>
+      </c>
+      <c r="N90" s="39">
+        <v>4</v>
+      </c>
+      <c r="O90" s="40">
+        <v>4</v>
+      </c>
+      <c r="Q90" s="40">
+        <v>4</v>
+      </c>
+      <c r="R90" s="39"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="21">
         <v>45</v>
       </c>
@@ -39849,11 +39963,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{203, 218}, </v>
       </c>
-      <c r="G91" s="21"/>
+      <c r="G91" s="21">
+        <v>4</v>
+      </c>
       <c r="H91" s="21"/>
-      <c r="I91" s="21"/>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I91" s="39">
+        <v>5</v>
+      </c>
+      <c r="J91" s="39">
+        <v>6</v>
+      </c>
+      <c r="K91" s="39">
+        <v>5</v>
+      </c>
+      <c r="L91" s="39">
+        <v>4</v>
+      </c>
+      <c r="M91" s="39">
+        <v>4</v>
+      </c>
+      <c r="N91" s="39">
+        <v>5</v>
+      </c>
+      <c r="O91" s="40">
+        <v>5</v>
+      </c>
+      <c r="Q91" s="40">
+        <v>5</v>
+      </c>
+      <c r="R91" s="39"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="21">
         <v>46</v>
       </c>
@@ -39867,11 +40007,36 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{204, 218}, </v>
       </c>
-      <c r="G92" s="21"/>
+      <c r="G92" s="21">
+        <v>5</v>
+      </c>
       <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I92" s="39">
+        <v>7</v>
+      </c>
+      <c r="J92" s="39">
+        <v>8</v>
+      </c>
+      <c r="K92" s="39">
+        <v>7</v>
+      </c>
+      <c r="L92" s="39">
+        <v>6</v>
+      </c>
+      <c r="M92" s="39">
+        <v>4</v>
+      </c>
+      <c r="N92" s="39">
+        <v>7</v>
+      </c>
+      <c r="O92" s="40">
+        <v>7</v>
+      </c>
+      <c r="Q92" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="21">
         <v>47</v>
       </c>
@@ -39885,11 +40050,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{204, 217}, </v>
       </c>
-      <c r="G93" s="21"/>
+      <c r="G93" s="21">
+        <v>7</v>
+      </c>
       <c r="H93" s="21"/>
-      <c r="I93" s="21"/>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I93" s="39">
+        <v>8</v>
+      </c>
+      <c r="J93" s="39">
+        <v>8</v>
+      </c>
+      <c r="K93" s="39">
+        <v>7</v>
+      </c>
+      <c r="L93" s="39">
+        <v>8</v>
+      </c>
+      <c r="M93" s="39">
+        <v>6</v>
+      </c>
+      <c r="N93" s="39">
+        <v>8</v>
+      </c>
+      <c r="O93" s="40">
+        <v>10</v>
+      </c>
+      <c r="Q93" s="40">
+        <v>10</v>
+      </c>
+      <c r="R93" s="39"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="21">
         <v>48</v>
       </c>
@@ -39903,11 +40094,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{207, 215}, </v>
       </c>
-      <c r="G94" s="21"/>
+      <c r="G94" s="21">
+        <v>10</v>
+      </c>
       <c r="H94" s="21"/>
-      <c r="I94" s="21"/>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I94" s="39">
+        <v>11</v>
+      </c>
+      <c r="J94" s="39">
+        <v>10</v>
+      </c>
+      <c r="K94" s="39">
+        <v>10</v>
+      </c>
+      <c r="L94" s="39">
+        <v>12</v>
+      </c>
+      <c r="M94" s="39">
+        <v>8</v>
+      </c>
+      <c r="N94" s="39">
+        <v>12</v>
+      </c>
+      <c r="O94" s="40">
+        <v>10</v>
+      </c>
+      <c r="Q94" s="40">
+        <v>10</v>
+      </c>
+      <c r="R94" s="39"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="21">
         <v>49</v>
       </c>
@@ -39921,11 +40138,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{208, 214}, </v>
       </c>
-      <c r="G95" s="21"/>
+      <c r="G95" s="21">
+        <v>12</v>
+      </c>
       <c r="H95" s="21"/>
-      <c r="I95" s="21"/>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I95" s="39">
+        <v>16</v>
+      </c>
+      <c r="J95" s="39">
+        <v>12</v>
+      </c>
+      <c r="K95" s="39">
+        <v>11</v>
+      </c>
+      <c r="L95" s="39">
+        <v>17</v>
+      </c>
+      <c r="M95" s="39">
+        <v>12</v>
+      </c>
+      <c r="N95" s="39">
+        <v>18</v>
+      </c>
+      <c r="O95" s="40">
+        <v>12</v>
+      </c>
+      <c r="Q95" s="40">
+        <v>12</v>
+      </c>
+      <c r="R95" s="39"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="21">
         <v>50</v>
       </c>
@@ -39939,11 +40182,36 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{209, 213}, </v>
       </c>
-      <c r="G96" s="21"/>
+      <c r="G96" s="21">
+        <v>16</v>
+      </c>
       <c r="H96" s="21"/>
-      <c r="I96" s="21"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I96" s="39">
+        <v>18</v>
+      </c>
+      <c r="J96" s="39">
+        <v>17</v>
+      </c>
+      <c r="K96" s="39">
+        <v>17</v>
+      </c>
+      <c r="L96" s="39">
+        <v>19</v>
+      </c>
+      <c r="M96" s="39">
+        <v>12</v>
+      </c>
+      <c r="N96" s="39">
+        <v>18</v>
+      </c>
+      <c r="O96" s="40">
+        <v>17</v>
+      </c>
+      <c r="Q96" s="40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="21">
         <v>51</v>
       </c>
@@ -39957,11 +40225,37 @@
         <f t="shared" si="26"/>
         <v xml:space="preserve">{210, 212}, </v>
       </c>
-      <c r="G97" s="21"/>
+      <c r="G97" s="21">
+        <v>17</v>
+      </c>
       <c r="H97" s="21"/>
-      <c r="I97" s="21"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I97" s="39">
+        <v>18</v>
+      </c>
+      <c r="J97" s="39">
+        <v>18</v>
+      </c>
+      <c r="K97" s="39">
+        <v>17</v>
+      </c>
+      <c r="L97" s="39">
+        <v>20</v>
+      </c>
+      <c r="M97" s="39">
+        <v>17</v>
+      </c>
+      <c r="N97" s="39">
+        <v>19</v>
+      </c>
+      <c r="O97" s="40">
+        <v>20</v>
+      </c>
+      <c r="Q97" s="40">
+        <v>19</v>
+      </c>
+      <c r="R97" s="39"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="21">
         <v>52</v>
       </c>
@@ -39972,32 +40266,259 @@
         <v>211</v>
       </c>
       <c r="E98" s="21" t="str">
-        <f t="shared" ref="E98" si="31">"{"&amp;B98&amp;", "&amp;C98&amp;"}"</f>
+        <f t="shared" ref="E98" si="32">"{"&amp;B98&amp;", "&amp;C98&amp;"}"</f>
         <v>{211, 211}</v>
       </c>
-      <c r="G98" s="21"/>
+      <c r="G98" s="21">
+        <v>21</v>
+      </c>
       <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I98" s="39">
+        <v>20</v>
+      </c>
+      <c r="J98" s="39">
+        <v>21</v>
+      </c>
+      <c r="K98" s="39">
+        <v>20</v>
+      </c>
+      <c r="L98" s="39">
+        <v>27</v>
+      </c>
+      <c r="M98" s="39">
+        <v>20</v>
+      </c>
+      <c r="N98" s="39">
+        <v>26</v>
+      </c>
+      <c r="O98" s="40">
+        <v>27</v>
+      </c>
+      <c r="Q98" s="40">
+        <v>26</v>
+      </c>
+      <c r="R98" s="39"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B99" s="21"/>
-      <c r="G99" s="21"/>
+      <c r="G99" s="21">
+        <v>21</v>
+      </c>
       <c r="H99" s="21"/>
-      <c r="I99" s="21"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G100" s="21"/>
+      <c r="I99" s="39">
+        <v>26</v>
+      </c>
+      <c r="J99" s="39">
+        <v>27</v>
+      </c>
+      <c r="K99" s="39">
+        <v>27</v>
+      </c>
+      <c r="L99" s="39">
+        <v>30</v>
+      </c>
+      <c r="M99" s="39">
+        <v>27</v>
+      </c>
+      <c r="N99" s="39">
+        <v>30</v>
+      </c>
+      <c r="O99" s="40">
+        <v>27</v>
+      </c>
+      <c r="Q99" s="40">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G100" s="21">
+        <v>30</v>
+      </c>
       <c r="H100" s="21"/>
-      <c r="I100" s="21"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G101" s="21"/>
+      <c r="I100" s="39">
+        <v>33</v>
+      </c>
+      <c r="J100" s="39">
+        <v>30</v>
+      </c>
+      <c r="K100" s="39">
+        <v>30</v>
+      </c>
+      <c r="L100" s="39">
+        <v>33</v>
+      </c>
+      <c r="M100" s="39">
+        <v>33</v>
+      </c>
+      <c r="N100" s="39">
+        <v>33</v>
+      </c>
+      <c r="O100" s="40">
+        <v>33</v>
+      </c>
+      <c r="Q100" s="40">
+        <v>33</v>
+      </c>
+      <c r="R100" s="39"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G101" s="21">
+        <v>33</v>
+      </c>
       <c r="H101" s="21"/>
-      <c r="I101" s="21"/>
+      <c r="I101" s="39">
+        <v>37</v>
+      </c>
+      <c r="J101" s="39">
+        <v>36</v>
+      </c>
+      <c r="K101" s="39">
+        <v>33</v>
+      </c>
+      <c r="L101" s="39">
+        <v>37</v>
+      </c>
+      <c r="M101" s="39">
+        <v>33</v>
+      </c>
+      <c r="N101" s="39">
+        <v>37</v>
+      </c>
+      <c r="O101" s="40">
+        <v>33</v>
+      </c>
+      <c r="Q101" s="40">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G102" s="21">
+        <v>37</v>
+      </c>
+      <c r="H102" s="21"/>
+      <c r="I102" s="39">
+        <v>43</v>
+      </c>
+      <c r="J102" s="39">
+        <v>40</v>
+      </c>
+      <c r="K102" s="39">
+        <v>37</v>
+      </c>
+      <c r="L102" s="39">
+        <v>41</v>
+      </c>
+      <c r="M102" s="39">
+        <v>37</v>
+      </c>
+      <c r="N102" s="39">
+        <v>43</v>
+      </c>
+      <c r="O102" s="40">
+        <v>41</v>
+      </c>
+      <c r="Q102" s="40">
+        <v>41</v>
+      </c>
+      <c r="R102" s="39"/>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G103" s="21">
+        <v>43</v>
+      </c>
+      <c r="H103" s="21"/>
+      <c r="I103" s="39">
+        <v>49</v>
+      </c>
+      <c r="J103" s="39">
+        <v>48</v>
+      </c>
+      <c r="K103" s="39">
+        <v>43</v>
+      </c>
+      <c r="L103" s="39">
+        <v>49</v>
+      </c>
+      <c r="M103" s="39">
+        <v>43</v>
+      </c>
+      <c r="N103" s="39">
+        <v>50</v>
+      </c>
+      <c r="O103" s="40">
+        <v>41</v>
+      </c>
+      <c r="Q103" s="40">
+        <v>49</v>
+      </c>
+      <c r="R103" s="39"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G104" s="21">
+        <v>49</v>
+      </c>
+      <c r="H104" s="21"/>
+      <c r="I104" s="39">
+        <v>51</v>
+      </c>
+      <c r="J104" s="39">
+        <v>50</v>
+      </c>
+      <c r="K104" s="39">
+        <v>50</v>
+      </c>
+      <c r="L104" s="39">
+        <v>49</v>
+      </c>
+      <c r="M104" s="39">
+        <v>50</v>
+      </c>
+      <c r="N104" s="39">
+        <v>50</v>
+      </c>
+      <c r="O104" s="40">
+        <v>49</v>
+      </c>
+      <c r="Q104" s="40">
+        <v>50</v>
+      </c>
+      <c r="R104" s="39"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>5241</v>
+      </c>
+      <c r="I105">
+        <v>5231</v>
+      </c>
+      <c r="J105" s="39">
+        <v>5253</v>
+      </c>
+      <c r="K105" s="39">
+        <v>5258</v>
+      </c>
+      <c r="L105" s="39">
+        <v>5262</v>
+      </c>
+      <c r="M105" s="39">
+        <v>5263</v>
+      </c>
+      <c r="N105" s="39">
+        <v>52636</v>
+      </c>
+      <c r="O105" s="40">
+        <v>5275</v>
+      </c>
+      <c r="Q105" s="39"/>
+      <c r="R105" s="39"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q106" s="39"/>
+      <c r="R106" s="39"/>
     </row>
   </sheetData>
-  <sortState ref="O44:O81">
-    <sortCondition descending="1" ref="O44"/>
+  <sortState ref="R87:R104">
+    <sortCondition ref="R87"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Final test with extinction, not needed, best solution = 132.52756426
</commit_message>
<xml_diff>
--- a/Project Euler problem 314.xlsx
+++ b/Project Euler problem 314.xlsx
@@ -837,11 +837,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262040960"/>
-        <c:axId val="262046848"/>
+        <c:axId val="316947072"/>
+        <c:axId val="316957056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262040960"/>
+        <c:axId val="316947072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,12 +852,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262046848"/>
+        <c:crossAx val="316957056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262046848"/>
+        <c:axId val="316957056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262040960"/>
+        <c:crossAx val="316947072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1211,11 +1211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289521024"/>
-        <c:axId val="289535104"/>
+        <c:axId val="317549184"/>
+        <c:axId val="317563264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289521024"/>
+        <c:axId val="317549184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="212"/>
@@ -1238,14 +1238,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289535104"/>
+        <c:crossAx val="317563264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289535104"/>
+        <c:axId val="317563264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1258,7 +1258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289521024"/>
+        <c:crossAx val="317549184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1831,11 +1831,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289607040"/>
-        <c:axId val="289629312"/>
+        <c:axId val="317581952"/>
+        <c:axId val="317587840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289607040"/>
+        <c:axId val="317581952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="213"/>
@@ -1858,14 +1858,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289629312"/>
+        <c:crossAx val="317587840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289629312"/>
+        <c:axId val="317587840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1878,7 +1878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289607040"/>
+        <c:crossAx val="317581952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2451,11 +2451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289645696"/>
-        <c:axId val="289647232"/>
+        <c:axId val="317620608"/>
+        <c:axId val="317622144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289645696"/>
+        <c:axId val="317620608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2478,14 +2478,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289647232"/>
+        <c:crossAx val="317622144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289647232"/>
+        <c:axId val="317622144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="211"/>
@@ -2498,7 +2498,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289645696"/>
+        <c:crossAx val="317620608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2744,11 +2744,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261861376"/>
-        <c:axId val="261862912"/>
+        <c:axId val="315661312"/>
+        <c:axId val="315687680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261861376"/>
+        <c:axId val="315661312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2759,12 +2759,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261862912"/>
+        <c:crossAx val="315687680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261862912"/>
+        <c:axId val="315687680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2775,7 +2775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261861376"/>
+        <c:crossAx val="315661312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3122,11 +3122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289737728"/>
-        <c:axId val="289747712"/>
+        <c:axId val="317647104"/>
+        <c:axId val="317648896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289737728"/>
+        <c:axId val="317647104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,12 +3137,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289747712"/>
+        <c:crossAx val="317648896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289747712"/>
+        <c:axId val="317648896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3153,7 +3153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289737728"/>
+        <c:crossAx val="317647104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3600,11 +3600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289774592"/>
-        <c:axId val="289776384"/>
+        <c:axId val="316147968"/>
+        <c:axId val="316157952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289774592"/>
+        <c:axId val="316147968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3615,12 +3615,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289776384"/>
+        <c:crossAx val="316157952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289776384"/>
+        <c:axId val="316157952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,7 +3631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289774592"/>
+        <c:crossAx val="316147968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4090,11 +4090,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289796864"/>
-        <c:axId val="289798400"/>
+        <c:axId val="316190720"/>
+        <c:axId val="316192256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289796864"/>
+        <c:axId val="316190720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4105,12 +4105,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289798400"/>
+        <c:crossAx val="316192256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289798400"/>
+        <c:axId val="316192256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4121,7 +4121,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289796864"/>
+        <c:crossAx val="316190720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4263,11 +4263,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="261973888"/>
-        <c:axId val="261975424"/>
+        <c:axId val="316281984"/>
+        <c:axId val="316283520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261973888"/>
+        <c:axId val="316281984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4276,7 +4276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261975424"/>
+        <c:crossAx val="316283520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4284,7 +4284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261975424"/>
+        <c:axId val="316283520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4296,7 +4296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261973888"/>
+        <c:crossAx val="316281984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4435,11 +4435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="261991040"/>
-        <c:axId val="262009216"/>
+        <c:axId val="316303232"/>
+        <c:axId val="316304768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261991040"/>
+        <c:axId val="316303232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4448,7 +4448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262009216"/>
+        <c:crossAx val="316304768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4456,7 +4456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262009216"/>
+        <c:axId val="316304768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4468,7 +4468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261991040"/>
+        <c:crossAx val="316303232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5039,11 +5039,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="290128640"/>
-        <c:axId val="290130176"/>
+        <c:axId val="317181952"/>
+        <c:axId val="317183488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="290128640"/>
+        <c:axId val="317181952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="214"/>
@@ -5066,14 +5066,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290130176"/>
+        <c:crossAx val="317183488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="290130176"/>
+        <c:axId val="317183488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -5086,7 +5086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290128640"/>
+        <c:crossAx val="317181952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -5482,11 +5482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262072192"/>
-        <c:axId val="262073728"/>
+        <c:axId val="316990592"/>
+        <c:axId val="316992128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262072192"/>
+        <c:axId val="316990592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5497,12 +5497,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262073728"/>
+        <c:crossAx val="316992128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262073728"/>
+        <c:axId val="316992128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,7 +5513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262072192"/>
+        <c:crossAx val="316990592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6060,11 +6060,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="261732608"/>
-        <c:axId val="290168832"/>
+        <c:axId val="317203968"/>
+        <c:axId val="317205504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261732608"/>
+        <c:axId val="317203968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="214"/>
@@ -6087,14 +6087,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290168832"/>
+        <c:crossAx val="317205504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="290168832"/>
+        <c:axId val="317205504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -6107,7 +6107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261732608"/>
+        <c:crossAx val="317203968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -6189,7 +6189,7 @@
                   <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>180</c:v>
@@ -6204,22 +6204,22 @@
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>210</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>212</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>214</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>220</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
@@ -6234,7 +6234,7 @@
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>237</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>237</c:v>
@@ -6312,7 +6312,7 @@
                   <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>237</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>234</c:v>
@@ -6327,22 +6327,22 @@
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>214</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>212</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>210</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>208</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>201</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>193</c:v>
@@ -6357,7 +6357,7 @@
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>174</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>174</c:v>
@@ -6440,7 +6440,7 @@
                   <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>180</c:v>
@@ -6455,22 +6455,22 @@
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>210</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>212</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>214</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>220</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
@@ -6485,7 +6485,7 @@
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>237</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>237</c:v>
@@ -6563,7 +6563,7 @@
                   <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>174</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>180</c:v>
@@ -6578,22 +6578,22 @@
                   <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>201</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>208</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>210</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>212</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>214</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>220</c:v>
+                  <c:v>223</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>226</c:v>
@@ -6608,7 +6608,7 @@
                   <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>237</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>237</c:v>
@@ -6656,11 +6656,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289972608"/>
-        <c:axId val="289974144"/>
+        <c:axId val="317689216"/>
+        <c:axId val="317691008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289972608"/>
+        <c:axId val="317689216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="215"/>
@@ -6683,14 +6683,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289974144"/>
+        <c:crossAx val="317691008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289974144"/>
+        <c:axId val="317691008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -6703,7 +6703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289972608"/>
+        <c:crossAx val="317689216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -6755,16 +6755,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>156</c:v>
@@ -6773,37 +6773,37 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>165</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>167</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>191</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>191</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>193</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>198</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>203</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>209</c:v>
@@ -6812,37 +6812,37 @@
                   <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>219</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>222</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>226</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>227</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>227</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>232</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>234</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>238</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>242</c:v>
@@ -6851,13 +6851,13 @@
                   <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>247</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>250</c:v>
@@ -6881,13 +6881,13 @@
                   <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>247</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>244</c:v>
@@ -6896,37 +6896,37 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>241</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>241</c:v>
+                  <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>240</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>238</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>234</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>232</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>227</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>227</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>226</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>222</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>219</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>213</c:v>
@@ -6935,37 +6935,37 @@
                   <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>203</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>198</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>193</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>191</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>191</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>184</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>180</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>172</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>167</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>165</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>165</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>162</c:v>
@@ -6974,16 +6974,16 @@
                   <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>156</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>145</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>140</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
@@ -7006,16 +7006,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>156</c:v>
@@ -7024,37 +7024,37 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>165</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>167</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>191</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>191</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>193</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>198</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>203</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>209</c:v>
@@ -7063,37 +7063,37 @@
                   <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>219</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>222</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>226</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>227</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>227</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>232</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>234</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>238</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>242</c:v>
@@ -7102,13 +7102,13 @@
                   <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>247</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>250</c:v>
@@ -7129,16 +7129,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>156</c:v>
@@ -7147,37 +7147,37 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>165</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>167</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>172</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>180</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>184</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>191</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>191</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>193</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>198</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>203</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>209</c:v>
@@ -7186,37 +7186,37 @@
                   <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>219</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>222</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>226</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>227</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>227</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>232</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>234</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>238</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>242</c:v>
@@ -7225,13 +7225,13 @@
                   <c:v>244</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>244</c:v>
+                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>247</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>250</c:v>
@@ -7252,11 +7252,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289879936"/>
-        <c:axId val="289881472"/>
+        <c:axId val="318055552"/>
+        <c:axId val="318057088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289879936"/>
+        <c:axId val="318055552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="214"/>
@@ -7279,14 +7279,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289881472"/>
+        <c:crossAx val="318057088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289881472"/>
+        <c:axId val="318057088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -7299,7 +7299,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289879936"/>
+        <c:crossAx val="318055552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -19378,11 +19378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289946624"/>
-        <c:axId val="290210560"/>
+        <c:axId val="318105856"/>
+        <c:axId val="318128128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289946624"/>
+        <c:axId val="318105856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -19405,14 +19405,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290210560"/>
+        <c:crossAx val="318128128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
         <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="290210560"/>
+        <c:axId val="318128128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -19425,7 +19425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289946624"/>
+        <c:crossAx val="318105856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -22491,11 +22491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="290287616"/>
-        <c:axId val="290289152"/>
+        <c:axId val="318159872"/>
+        <c:axId val="318169856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290287616"/>
+        <c:axId val="318159872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22515,7 +22515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290289152"/>
+        <c:crossAx val="318169856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22525,7 +22525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290289152"/>
+        <c:axId val="318169856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22536,7 +22536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290287616"/>
+        <c:crossAx val="318159872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22721,11 +22721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262640768"/>
-        <c:axId val="262642304"/>
+        <c:axId val="316881536"/>
+        <c:axId val="316887424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262640768"/>
+        <c:axId val="316881536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22736,12 +22736,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262642304"/>
+        <c:crossAx val="316887424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262642304"/>
+        <c:axId val="316887424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22752,7 +22752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262640768"/>
+        <c:crossAx val="316881536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23098,11 +23098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262676864"/>
-        <c:axId val="262678400"/>
+        <c:axId val="316913536"/>
+        <c:axId val="316915072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262676864"/>
+        <c:axId val="316913536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23113,12 +23113,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262678400"/>
+        <c:crossAx val="316915072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262678400"/>
+        <c:axId val="316915072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23129,7 +23129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262676864"/>
+        <c:crossAx val="316913536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23642,11 +23642,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262701824"/>
-        <c:axId val="262703360"/>
+        <c:axId val="316930304"/>
+        <c:axId val="317267968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262701824"/>
+        <c:axId val="316930304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -23659,12 +23659,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262703360"/>
+        <c:crossAx val="317267968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262703360"/>
+        <c:axId val="317267968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -23677,7 +23677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262701824"/>
+        <c:crossAx val="316930304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24129,11 +24129,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262727168"/>
-        <c:axId val="262728704"/>
+        <c:axId val="317301504"/>
+        <c:axId val="317303040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="262727168"/>
+        <c:axId val="317301504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24144,12 +24144,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262728704"/>
+        <c:crossAx val="317303040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="262728704"/>
+        <c:axId val="317303040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24160,7 +24160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262727168"/>
+        <c:crossAx val="317301504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24519,11 +24519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289440512"/>
-        <c:axId val="289442048"/>
+        <c:axId val="317341696"/>
+        <c:axId val="317343232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289440512"/>
+        <c:axId val="317341696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24534,12 +24534,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289442048"/>
+        <c:crossAx val="317343232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289442048"/>
+        <c:axId val="317343232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24550,7 +24550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289440512"/>
+        <c:crossAx val="317341696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24713,11 +24713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="289464320"/>
-        <c:axId val="289465856"/>
+        <c:axId val="317348864"/>
+        <c:axId val="317371136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="289464320"/>
+        <c:axId val="317348864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24726,7 +24726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289465856"/>
+        <c:crossAx val="317371136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24734,7 +24734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289465856"/>
+        <c:axId val="317371136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -24746,7 +24746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289464320"/>
+        <c:crossAx val="317348864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -24918,11 +24918,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="289480704"/>
-        <c:axId val="289482240"/>
+        <c:axId val="317377920"/>
+        <c:axId val="317523072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="289480704"/>
+        <c:axId val="317377920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24931,7 +24931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289482240"/>
+        <c:crossAx val="317523072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -24939,7 +24939,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289482240"/>
+        <c:axId val="317523072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24950,7 +24950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="289480704"/>
+        <c:crossAx val="317377920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -51549,7 +51549,7 @@
   <dimension ref="A1:AF104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51632,7 +51632,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="26">
-        <f>VLOOKUP(G3,xy_lut,2,FALSE)</f>
+        <f t="shared" ref="H3:H20" si="2">VLOOKUP(G3,xy_lut,2,FALSE)</f>
         <v>122</v>
       </c>
       <c r="I3" s="27">
@@ -51643,7 +51643,7 @@
         <v>122</v>
       </c>
       <c r="K3" s="21">
-        <f t="shared" ref="K3:K11" si="2">SQRT((H2-H3)^2+(I2-I3)^2)</f>
+        <f t="shared" ref="K3:K11" si="3">SQRT((H2-H3)^2+(I2-I3)^2)</f>
         <v>122</v>
       </c>
       <c r="L3" s="21">
@@ -51670,11 +51670,11 @@
         <v>1</v>
       </c>
       <c r="H4" s="28">
-        <f>VLOOKUP(G4,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="I4" s="29">
-        <f>VLOOKUP(G4,xy_lut,3,FALSE)</f>
+        <f t="shared" ref="I4:I20" si="4">VLOOKUP(G4,xy_lut,3,FALSE)</f>
         <v>249</v>
       </c>
       <c r="J4" s="21">
@@ -51682,7 +51682,7 @@
         <v>133</v>
       </c>
       <c r="K4" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.045361017187261</v>
       </c>
       <c r="L4" s="21">
@@ -51709,11 +51709,11 @@
         <v>3</v>
       </c>
       <c r="H5" s="28">
-        <f>VLOOKUP(G5,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="I5" s="29">
-        <f>VLOOKUP(G5,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>248</v>
       </c>
       <c r="J5" s="21">
@@ -51721,11 +51721,11 @@
         <v>140</v>
       </c>
       <c r="K5" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.0710678118654755</v>
       </c>
       <c r="L5" s="21">
-        <f t="shared" ref="L5:L26" si="3">(H5-H4)*(I4+I5)/2</f>
+        <f t="shared" ref="L5:L26" si="5">(H5-H4)*(I4+I5)/2</f>
         <v>1739.5</v>
       </c>
       <c r="O5" s="21"/>
@@ -51748,11 +51748,11 @@
         <v>4</v>
       </c>
       <c r="H6" s="28">
-        <f>VLOOKUP(G6,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
       <c r="I6" s="29">
-        <f>VLOOKUP(G6,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>247</v>
       </c>
       <c r="J6" s="21">
@@ -51760,11 +51760,11 @@
         <v>145</v>
       </c>
       <c r="K6" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.0990195135927845</v>
       </c>
       <c r="L6" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1237.5</v>
       </c>
       <c r="O6" s="21"/>
@@ -51787,11 +51787,11 @@
         <v>5</v>
       </c>
       <c r="H7" s="28">
-        <f>VLOOKUP(G7,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>149</v>
       </c>
       <c r="I7" s="29">
-        <f>VLOOKUP(G7,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>246</v>
       </c>
       <c r="J7" s="21">
@@ -51799,11 +51799,11 @@
         <v>149</v>
       </c>
       <c r="K7" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.1231056256176606</v>
       </c>
       <c r="L7" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>986</v>
       </c>
       <c r="O7" s="21"/>
@@ -51826,11 +51826,11 @@
         <v>7</v>
       </c>
       <c r="H8" s="28">
-        <f>VLOOKUP(G8,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="I8" s="29">
-        <f>VLOOKUP(G8,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>244</v>
       </c>
       <c r="J8" s="21">
@@ -51838,11 +51838,11 @@
         <v>156</v>
       </c>
       <c r="K8" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.2801098892805181</v>
       </c>
       <c r="L8" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1715</v>
       </c>
       <c r="O8" s="21"/>
@@ -51865,11 +51865,11 @@
         <v>8</v>
       </c>
       <c r="H9" s="28">
-        <f>VLOOKUP(G9,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="I9" s="29">
-        <f>VLOOKUP(G9,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>243</v>
       </c>
       <c r="J9" s="21">
@@ -51877,11 +51877,11 @@
         <v>159</v>
       </c>
       <c r="K9" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1622776601683795</v>
       </c>
       <c r="L9" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>730.5</v>
       </c>
       <c r="O9" s="21"/>
@@ -51904,11 +51904,11 @@
         <v>10</v>
       </c>
       <c r="H10" s="28">
-        <f>VLOOKUP(G10,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>162</v>
       </c>
       <c r="I10" s="29">
-        <f>VLOOKUP(G10,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
       <c r="J10" s="21">
@@ -51916,11 +51916,11 @@
         <v>162</v>
       </c>
       <c r="K10" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1622776601683795</v>
       </c>
       <c r="L10" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>727.5</v>
       </c>
       <c r="O10" s="21"/>
@@ -51943,11 +51943,11 @@
         <v>12</v>
       </c>
       <c r="H11" s="28">
-        <f>VLOOKUP(G11,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="I11" s="29">
-        <f>VLOOKUP(G11,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="J11" s="21">
@@ -51955,11 +51955,11 @@
         <v>167</v>
       </c>
       <c r="K11" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.3851648071345037</v>
       </c>
       <c r="L11" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1205</v>
       </c>
       <c r="O11" s="21"/>
@@ -51982,11 +51982,11 @@
         <v>17</v>
       </c>
       <c r="H12" s="28">
-        <f>VLOOKUP(G12,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="I12" s="29">
-        <f>VLOOKUP(G12,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>237</v>
       </c>
       <c r="J12" s="21">
@@ -51998,7 +51998,7 @@
         <v>7.6157731058639087</v>
       </c>
       <c r="L12" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1669.5</v>
       </c>
       <c r="O12" s="21"/>
@@ -52018,27 +52018,27 @@
         <v xml:space="preserve">{165, 241}, </v>
       </c>
       <c r="G13" s="43">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H13" s="28">
-        <f>VLOOKUP(G13,xy_lut,2,FALSE)</f>
-        <v>174</v>
+        <f t="shared" si="2"/>
+        <v>176</v>
       </c>
       <c r="I13" s="29">
-        <f>VLOOKUP(G13,xy_lut,3,FALSE)</f>
-        <v>237</v>
+        <f t="shared" si="4"/>
+        <v>236</v>
       </c>
       <c r="J13" s="21">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K13" s="21">
-        <f t="shared" ref="K13:K39" si="4">SQRT((H12-H13)^2+(I12-I13)^2)</f>
-        <v>0</v>
+        <f t="shared" ref="K13:K39" si="6">SQRT((H12-H13)^2+(I12-I13)^2)</f>
+        <v>2.2360679774997898</v>
       </c>
       <c r="L13" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>473</v>
       </c>
       <c r="O13" s="21"/>
     </row>
@@ -52060,11 +52060,11 @@
         <v>20</v>
       </c>
       <c r="H14" s="28">
-        <f>VLOOKUP(G14,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>180</v>
       </c>
       <c r="I14" s="29">
-        <f>VLOOKUP(G14,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>234</v>
       </c>
       <c r="J14" s="21">
@@ -52072,12 +52072,12 @@
         <v>180</v>
       </c>
       <c r="K14" s="21">
-        <f t="shared" si="4"/>
-        <v>6.7082039324993694</v>
+        <f t="shared" si="6"/>
+        <v>4.4721359549995796</v>
       </c>
       <c r="L14" s="21">
-        <f t="shared" si="3"/>
-        <v>1413</v>
+        <f t="shared" si="5"/>
+        <v>940</v>
       </c>
       <c r="O14" s="21"/>
     </row>
@@ -52099,11 +52099,11 @@
         <v>27</v>
       </c>
       <c r="H15" s="28">
-        <f>VLOOKUP(G15,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>187</v>
       </c>
       <c r="I15" s="29">
-        <f>VLOOKUP(G15,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>230</v>
       </c>
       <c r="J15" s="21">
@@ -52111,11 +52111,11 @@
         <v>187</v>
       </c>
       <c r="K15" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.0622577482985491</v>
       </c>
       <c r="L15" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1624</v>
       </c>
       <c r="O15" s="21"/>
@@ -52138,11 +52138,11 @@
         <v>30</v>
       </c>
       <c r="H16" s="28">
-        <f>VLOOKUP(G16,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>190</v>
       </c>
       <c r="I16" s="29">
-        <f>VLOOKUP(G16,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="J16" s="21">
@@ -52150,11 +52150,11 @@
         <v>190</v>
       </c>
       <c r="K16" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6055512754639891</v>
       </c>
       <c r="L16" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>687</v>
       </c>
       <c r="O16" s="21"/>
@@ -52177,11 +52177,11 @@
         <v>33</v>
       </c>
       <c r="H17" s="28">
-        <f>VLOOKUP(G17,xy_lut,2,FALSE)</f>
+        <f t="shared" si="2"/>
         <v>193</v>
       </c>
       <c r="I17" s="29">
-        <f>VLOOKUP(G17,xy_lut,3,FALSE)</f>
+        <f t="shared" si="4"/>
         <v>226</v>
       </c>
       <c r="J17" s="21">
@@ -52189,11 +52189,11 @@
         <v>193</v>
       </c>
       <c r="K17" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6055512754639891</v>
       </c>
       <c r="L17" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>681</v>
       </c>
       <c r="O17" s="21"/>
@@ -52213,27 +52213,27 @@
         <v xml:space="preserve">{172, 238}, </v>
       </c>
       <c r="G18" s="43">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H18" s="28">
-        <f>VLOOKUP(G18,xy_lut,2,FALSE)</f>
-        <v>201</v>
+        <f t="shared" si="2"/>
+        <v>197</v>
       </c>
       <c r="I18" s="29">
-        <f>VLOOKUP(G18,xy_lut,3,FALSE)</f>
-        <v>220</v>
+        <f t="shared" si="4"/>
+        <v>223</v>
       </c>
       <c r="J18" s="21">
         <f t="shared" si="1"/>
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="K18" s="21">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="L18" s="21">
-        <f t="shared" si="3"/>
-        <v>1784</v>
+        <f t="shared" si="5"/>
+        <v>898</v>
       </c>
       <c r="O18" s="21"/>
     </row>
@@ -52252,27 +52252,27 @@
         <v xml:space="preserve">{174, 237}, </v>
       </c>
       <c r="G19" s="43">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H19" s="28">
-        <f>VLOOKUP(G19,xy_lut,2,FALSE)</f>
-        <v>208</v>
+        <f t="shared" si="2"/>
+        <v>201</v>
       </c>
       <c r="I19" s="29">
-        <f>VLOOKUP(G19,xy_lut,3,FALSE)</f>
-        <v>214</v>
+        <f t="shared" si="4"/>
+        <v>220</v>
       </c>
       <c r="J19" s="21">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K19" s="21">
-        <f t="shared" si="4"/>
-        <v>9.2195444572928871</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="L19" s="21">
-        <f t="shared" si="3"/>
-        <v>1519</v>
+        <f t="shared" si="5"/>
+        <v>886</v>
       </c>
       <c r="O19" s="21"/>
     </row>
@@ -52291,27 +52291,27 @@
         <v xml:space="preserve">{176, 236}, </v>
       </c>
       <c r="G20" s="43">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" s="30">
-        <f>VLOOKUP(G20,xy_lut,2,FALSE)</f>
-        <v>210</v>
+        <f t="shared" si="2"/>
+        <v>208</v>
       </c>
       <c r="I20" s="31">
-        <f>VLOOKUP(G20,xy_lut,3,FALSE)</f>
-        <v>212</v>
+        <f t="shared" si="4"/>
+        <v>214</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K20" s="21">
-        <f t="shared" si="4"/>
-        <v>2.8284271247461903</v>
+        <f t="shared" si="6"/>
+        <v>9.2195444572928871</v>
       </c>
       <c r="L20" s="21">
-        <f t="shared" si="3"/>
-        <v>426</v>
+        <f t="shared" si="5"/>
+        <v>1519</v>
       </c>
       <c r="O20" s="21"/>
     </row>
@@ -52332,23 +52332,23 @@
       <c r="G21" s="21"/>
       <c r="H21" s="32">
         <f>I20</f>
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="I21" s="33">
         <f>H20</f>
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J21" s="21">
         <f t="shared" si="1"/>
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="K21" s="21">
-        <f t="shared" si="4"/>
-        <v>2.8284271247461903</v>
+        <f t="shared" si="6"/>
+        <v>8.4852813742385695</v>
       </c>
       <c r="L21" s="21">
-        <f t="shared" si="3"/>
-        <v>422</v>
+        <f t="shared" si="5"/>
+        <v>1266</v>
       </c>
       <c r="O21" s="21"/>
     </row>
@@ -52369,23 +52369,23 @@
       <c r="G22" s="21"/>
       <c r="H22" s="34">
         <f>I19</f>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="I22" s="35">
         <f>H19</f>
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="J22" s="21">
         <f t="shared" si="1"/>
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="K22" s="21">
-        <f t="shared" si="4"/>
-        <v>2.8284271247461903</v>
+        <f t="shared" si="6"/>
+        <v>9.2195444572928871</v>
       </c>
       <c r="L22" s="21">
-        <f t="shared" si="3"/>
-        <v>418</v>
+        <f t="shared" si="5"/>
+        <v>1227</v>
       </c>
       <c r="O22" s="21"/>
     </row>
@@ -52406,23 +52406,23 @@
       <c r="G23" s="21"/>
       <c r="H23" s="34">
         <f>I18</f>
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="I23" s="35">
         <f>H18</f>
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J23" s="21">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="K23" s="21">
-        <f t="shared" si="4"/>
-        <v>9.2195444572928871</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="L23" s="21">
-        <f t="shared" si="3"/>
-        <v>1227</v>
+        <f t="shared" si="5"/>
+        <v>597</v>
       </c>
       <c r="O23" s="21"/>
     </row>
@@ -52454,12 +52454,12 @@
         <v>226</v>
       </c>
       <c r="K24" s="21">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="L24" s="21">
-        <f t="shared" si="3"/>
-        <v>1182</v>
+        <f t="shared" si="5"/>
+        <v>585</v>
       </c>
       <c r="O24" s="21"/>
     </row>
@@ -52491,11 +52491,11 @@
         <v>228</v>
       </c>
       <c r="K25" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6055512754639891</v>
       </c>
       <c r="L25" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>383</v>
       </c>
       <c r="O25" s="21"/>
@@ -52528,11 +52528,11 @@
         <v>230</v>
       </c>
       <c r="K26" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.6055512754639891</v>
       </c>
       <c r="L26" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>377</v>
       </c>
       <c r="O26" s="21"/>
@@ -52565,7 +52565,7 @@
         <v>234</v>
       </c>
       <c r="K27" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.0622577482985491</v>
       </c>
       <c r="L27" s="21">
@@ -52591,23 +52591,23 @@
       <c r="G28" s="21"/>
       <c r="H28" s="34">
         <f>I13</f>
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I28" s="35">
         <f>H13</f>
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J28" s="21">
         <f t="shared" si="1"/>
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K28" s="21">
-        <f t="shared" si="4"/>
-        <v>6.7082039324993694</v>
+        <f t="shared" si="6"/>
+        <v>4.4721359549995796</v>
       </c>
       <c r="L28" s="21">
-        <f t="shared" ref="L28:L39" si="5">(H28-H27)*(I27+I28)/2</f>
-        <v>531</v>
+        <f t="shared" ref="L28:L39" si="7">(H28-H27)*(I27+I28)/2</f>
+        <v>356</v>
       </c>
       <c r="O28" s="21"/>
     </row>
@@ -52639,12 +52639,12 @@
         <v>237</v>
       </c>
       <c r="K29" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.2360679774997898</v>
       </c>
       <c r="L29" s="21">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>175</v>
       </c>
       <c r="O29" s="21"/>
     </row>
@@ -52676,11 +52676,11 @@
         <v>240</v>
       </c>
       <c r="K30" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.6157731058639087</v>
       </c>
       <c r="L30" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>511.5</v>
       </c>
       <c r="O30" s="21"/>
@@ -52713,11 +52713,11 @@
         <v>242</v>
       </c>
       <c r="K31" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.3851648071345037</v>
       </c>
       <c r="L31" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>329</v>
       </c>
       <c r="O31" s="21"/>
@@ -52750,11 +52750,11 @@
         <v>243</v>
       </c>
       <c r="K32" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.1622776601683795</v>
       </c>
       <c r="L32" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>160.5</v>
       </c>
       <c r="O32" s="21"/>
@@ -52787,11 +52787,11 @@
         <v>244</v>
       </c>
       <c r="K33" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.1622776601683795</v>
       </c>
       <c r="L33" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>157.5</v>
       </c>
       <c r="O33" s="21"/>
@@ -52807,7 +52807,7 @@
         <v>227</v>
       </c>
       <c r="D34" s="21" t="str">
-        <f t="shared" ref="D34:D53" si="6">"{"&amp;B34&amp;", "&amp;C34&amp;"}, "</f>
+        <f t="shared" ref="D34:D53" si="8">"{"&amp;B34&amp;", "&amp;C34&amp;"}, "</f>
         <v xml:space="preserve">{191, 227}, </v>
       </c>
       <c r="G34" s="21"/>
@@ -52824,11 +52824,11 @@
         <v>246</v>
       </c>
       <c r="K34" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.2801098892805181</v>
       </c>
       <c r="L34" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="O34" s="21"/>
@@ -52844,7 +52844,7 @@
         <v>226</v>
       </c>
       <c r="D35" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{193, 226}, </v>
       </c>
       <c r="G35" s="21"/>
@@ -52861,11 +52861,11 @@
         <v>247</v>
       </c>
       <c r="K35" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.1231056256176606</v>
       </c>
       <c r="L35" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>147</v>
       </c>
       <c r="O35" s="21"/>
@@ -52881,7 +52881,7 @@
         <v>226</v>
       </c>
       <c r="D36" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{194, 226}, </v>
       </c>
       <c r="G36" s="21"/>
@@ -52898,11 +52898,11 @@
         <v>248</v>
       </c>
       <c r="K36" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5.0990195135927845</v>
       </c>
       <c r="L36" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>142.5</v>
       </c>
       <c r="O36" s="21"/>
@@ -52918,7 +52918,7 @@
         <v>225</v>
       </c>
       <c r="D37" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{194, 225}, </v>
       </c>
       <c r="G37" s="21"/>
@@ -52935,11 +52935,11 @@
         <v>249</v>
       </c>
       <c r="K37" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.0710678118654755</v>
       </c>
       <c r="L37" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>136.5</v>
       </c>
       <c r="O37" s="21"/>
@@ -52955,7 +52955,7 @@
         <v>224</v>
       </c>
       <c r="D38" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{196, 224}, </v>
       </c>
       <c r="G38" s="21"/>
@@ -52972,11 +52972,11 @@
         <v>250</v>
       </c>
       <c r="K38" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11.045361017187261</v>
       </c>
       <c r="L38" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>127.5</v>
       </c>
     </row>
@@ -52991,7 +52991,7 @@
         <v>223</v>
       </c>
       <c r="D39" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{197, 223}, </v>
       </c>
       <c r="G39" s="21"/>
@@ -53008,11 +53008,11 @@
         <v>250</v>
       </c>
       <c r="K39" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>122</v>
       </c>
       <c r="L39" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -53027,7 +53027,7 @@
         <v>223</v>
       </c>
       <c r="D40" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{198, 223}, </v>
       </c>
       <c r="K40" s="21"/>
@@ -53044,12 +53044,12 @@
         <v>222</v>
       </c>
       <c r="D41" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{198, 222}, </v>
       </c>
       <c r="K41" s="21">
         <f>SUM(K3:K39)</f>
-        <v>442.77581293403392</v>
+        <v>442.77581293403398</v>
       </c>
       <c r="L41" s="21">
         <f>SUM(L3:L39)</f>
@@ -53071,7 +53071,7 @@
         <v>221</v>
       </c>
       <c r="D42" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{200, 221}, </v>
       </c>
     </row>
@@ -53086,7 +53086,7 @@
         <v>220</v>
       </c>
       <c r="D43" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{201, 220}, </v>
       </c>
       <c r="G43" s="41">
@@ -53095,7 +53095,7 @@
       <c r="H43" s="41">
         <v>0</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I43" s="41">
         <v>0</v>
       </c>
       <c r="J43" s="38">
@@ -53179,7 +53179,7 @@
         <v>220</v>
       </c>
       <c r="D44" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{202, 220}, </v>
       </c>
       <c r="G44" s="41">
@@ -53188,8 +53188,8 @@
       <c r="H44" s="41">
         <v>1</v>
       </c>
-      <c r="I44" s="38">
-        <v>0</v>
+      <c r="I44" s="41">
+        <v>1</v>
       </c>
       <c r="J44" s="38">
         <v>1</v>
@@ -53272,7 +53272,7 @@
         <v>219</v>
       </c>
       <c r="D45" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{202, 219}, </v>
       </c>
       <c r="G45" s="41">
@@ -53281,8 +53281,8 @@
       <c r="H45" s="41">
         <v>3</v>
       </c>
-      <c r="I45" s="38">
-        <v>0</v>
+      <c r="I45" s="41">
+        <v>3</v>
       </c>
       <c r="J45" s="38">
         <v>1</v>
@@ -53365,7 +53365,7 @@
         <v>219</v>
       </c>
       <c r="D46" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{203, 219}, </v>
       </c>
       <c r="G46" s="43">
@@ -53374,8 +53374,8 @@
       <c r="H46" s="43">
         <v>4</v>
       </c>
-      <c r="I46" s="38">
-        <v>1</v>
+      <c r="I46" s="43">
+        <v>4</v>
       </c>
       <c r="J46" s="38">
         <v>1</v>
@@ -53458,7 +53458,7 @@
         <v>218</v>
       </c>
       <c r="D47" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{203, 218}, </v>
       </c>
       <c r="G47" s="43">
@@ -53467,8 +53467,8 @@
       <c r="H47" s="43">
         <v>5</v>
       </c>
-      <c r="I47" s="38">
-        <v>3</v>
+      <c r="I47" s="43">
+        <v>5</v>
       </c>
       <c r="J47" s="38">
         <v>3</v>
@@ -53551,7 +53551,7 @@
         <v>218</v>
       </c>
       <c r="D48" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{204, 218}, </v>
       </c>
       <c r="G48" s="43">
@@ -53560,8 +53560,8 @@
       <c r="H48" s="43">
         <v>7</v>
       </c>
-      <c r="I48" s="38">
-        <v>3</v>
+      <c r="I48" s="43">
+        <v>7</v>
       </c>
       <c r="J48" s="38">
         <v>3</v>
@@ -53644,7 +53644,7 @@
         <v>217</v>
       </c>
       <c r="D49" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{204, 217}, </v>
       </c>
       <c r="G49" s="43">
@@ -53653,8 +53653,8 @@
       <c r="H49" s="43">
         <v>10</v>
       </c>
-      <c r="I49" s="38">
-        <v>3</v>
+      <c r="I49" s="43">
+        <v>8</v>
       </c>
       <c r="J49" s="38">
         <v>4</v>
@@ -53737,7 +53737,7 @@
         <v>215</v>
       </c>
       <c r="D50" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{207, 215}, </v>
       </c>
       <c r="G50" s="43">
@@ -53746,8 +53746,8 @@
       <c r="H50" s="43">
         <v>12</v>
       </c>
-      <c r="I50" s="38">
-        <v>7</v>
+      <c r="I50" s="43">
+        <v>10</v>
       </c>
       <c r="J50" s="38">
         <v>5</v>
@@ -53830,7 +53830,7 @@
         <v>214</v>
       </c>
       <c r="D51" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{208, 214}, </v>
       </c>
       <c r="G51" s="43">
@@ -53839,7 +53839,7 @@
       <c r="H51" s="43">
         <v>17</v>
       </c>
-      <c r="I51" s="38">
+      <c r="I51" s="43">
         <v>12</v>
       </c>
       <c r="J51" s="38">
@@ -53923,7 +53923,7 @@
         <v>213</v>
       </c>
       <c r="D52" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{209, 213}, </v>
       </c>
       <c r="G52" s="43">
@@ -53932,8 +53932,8 @@
       <c r="H52" s="43">
         <v>18</v>
       </c>
-      <c r="I52" s="38">
-        <v>16</v>
+      <c r="I52" s="43">
+        <v>17</v>
       </c>
       <c r="J52" s="38">
         <v>10</v>
@@ -54016,7 +54016,7 @@
         <v>212</v>
       </c>
       <c r="D53" s="21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">{210, 212}, </v>
       </c>
       <c r="G53" s="43">
@@ -54025,8 +54025,8 @@
       <c r="H53" s="43">
         <v>20</v>
       </c>
-      <c r="I53" s="38">
-        <v>18</v>
+      <c r="I53" s="43">
+        <v>17</v>
       </c>
       <c r="J53" s="38">
         <v>12</v>
@@ -54118,8 +54118,8 @@
       <c r="H54" s="43">
         <v>27</v>
       </c>
-      <c r="I54" s="38">
-        <v>18</v>
+      <c r="I54" s="43">
+        <v>20</v>
       </c>
       <c r="J54" s="38">
         <v>15</v>
@@ -54199,8 +54199,8 @@
       <c r="H55" s="43">
         <v>30</v>
       </c>
-      <c r="I55" s="38">
-        <v>26</v>
+      <c r="I55" s="43">
+        <v>27</v>
       </c>
       <c r="J55" s="38">
         <v>18</v>
@@ -54279,8 +54279,8 @@
       <c r="H56" s="43">
         <v>33</v>
       </c>
-      <c r="I56" s="38">
-        <v>33</v>
+      <c r="I56" s="43">
+        <v>30</v>
       </c>
       <c r="J56" s="38">
         <v>26</v>
@@ -54359,8 +54359,8 @@
       <c r="H57" s="43">
         <v>37</v>
       </c>
-      <c r="I57" s="38">
-        <v>35</v>
+      <c r="I57" s="43">
+        <v>33</v>
       </c>
       <c r="J57" s="38">
         <v>33</v>
@@ -54439,8 +54439,8 @@
       <c r="H58" s="43">
         <v>41</v>
       </c>
-      <c r="I58" s="38">
-        <v>40</v>
+      <c r="I58" s="43">
+        <v>41</v>
       </c>
       <c r="J58" s="38">
         <v>40</v>
@@ -54519,8 +54519,8 @@
       <c r="H59" s="43">
         <v>49</v>
       </c>
-      <c r="I59" s="38">
-        <v>48</v>
+      <c r="I59" s="43">
+        <v>49</v>
       </c>
       <c r="J59" s="38">
         <v>48</v>
@@ -54599,7 +54599,7 @@
       <c r="H60" s="43">
         <v>49</v>
       </c>
-      <c r="I60" s="38">
+      <c r="I60" s="43">
         <v>51</v>
       </c>
       <c r="J60" s="38">
@@ -54680,7 +54680,7 @@
         <v>132.52756425686314</v>
       </c>
       <c r="I61" s="44">
-        <v>132.498696499</v>
+        <v>132.52756425686314</v>
       </c>
       <c r="J61" s="44">
         <v>132.51827352800001</v>
@@ -54797,7 +54797,7 @@
         <v>250</v>
       </c>
       <c r="J65" s="21">
-        <f t="shared" ref="J65:J66" si="7">H65</f>
+        <f t="shared" ref="J65:J66" si="9">H65</f>
         <v>0</v>
       </c>
       <c r="K65" s="21"/>
@@ -54818,34 +54818,34 @@
       </c>
       <c r="E66">
         <f ca="1">RAND()/2</f>
-        <v>0.36394129051605162</v>
+        <v>0.13309531200671137</v>
       </c>
       <c r="F66">
         <f ca="1">E66</f>
-        <v>0.36394129051605162</v>
+        <v>0.13309531200671137</v>
       </c>
       <c r="G66">
-        <f ca="1">ROUND(52*F66/F$84,0)</f>
-        <v>3</v>
+        <f t="shared" ref="G66:G84" ca="1" si="10">ROUND(52*F66/F$84,0)</f>
+        <v>1</v>
       </c>
       <c r="H66" s="26">
-        <f t="shared" ref="H66:H83" ca="1" si="8">VLOOKUP(G66,xy_lut,2,FALSE)</f>
-        <v>140</v>
+        <f t="shared" ref="H66:H83" ca="1" si="11">VLOOKUP(G66,xy_lut,2,FALSE)</f>
+        <v>133</v>
       </c>
       <c r="I66" s="27">
         <v>250</v>
       </c>
       <c r="J66" s="21">
-        <f t="shared" ca="1" si="7"/>
-        <v>140</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>133</v>
       </c>
       <c r="K66" s="21">
-        <f t="shared" ref="K66" ca="1" si="9">SQRT((H65-H66)^2+(I65-I66)^2)</f>
-        <v>140</v>
+        <f t="shared" ref="K66" ca="1" si="12">SQRT((H65-H66)^2+(I65-I66)^2)</f>
+        <v>133</v>
       </c>
       <c r="L66" s="21">
         <f ca="1">H66*I66</f>
-        <v>35000</v>
+        <v>33250</v>
       </c>
       <c r="M66" s="21">
         <v>1</v>
@@ -54862,36 +54862,36 @@
         <v>2</v>
       </c>
       <c r="E67" s="21">
-        <f t="shared" ref="E67:E73" ca="1" si="10">RAND()/2</f>
-        <v>0.15040332067855838</v>
+        <f t="shared" ref="E67:E73" ca="1" si="13">RAND()/2</f>
+        <v>0.20681942030895895</v>
       </c>
       <c r="F67">
         <f ca="1">F66+E67</f>
-        <v>0.51434461119460995</v>
+        <v>0.33991473231567032</v>
       </c>
       <c r="G67" s="21">
-        <f ca="1">ROUND(52*F67/F$84,0)</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2</v>
       </c>
       <c r="H67" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>145</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>134</v>
       </c>
       <c r="I67" s="29">
-        <f t="shared" ref="I67:I83" ca="1" si="11">VLOOKUP(G67,xy_lut,3,FALSE)</f>
-        <v>247</v>
+        <f t="shared" ref="I67:I83" ca="1" si="14">VLOOKUP(G67,xy_lut,3,FALSE)</f>
+        <v>249</v>
       </c>
       <c r="J67" s="21">
-        <f t="shared" ref="J67:J74" ca="1" si="12">H67</f>
-        <v>145</v>
+        <f t="shared" ref="J67:J74" ca="1" si="15">H67</f>
+        <v>134</v>
       </c>
       <c r="K67" s="21">
-        <f t="shared" ref="K67:K74" ca="1" si="13">SQRT((H66-H67)^2+(I66-I67)^2)</f>
-        <v>5.8309518948453007</v>
+        <f t="shared" ref="K67:K74" ca="1" si="16">SQRT((H66-H67)^2+(I66-I67)^2)</f>
+        <v>1.4142135623730951</v>
       </c>
       <c r="L67" s="21">
         <f ca="1">(H67-H66)*(I66+I67)/2</f>
-        <v>1242.5</v>
+        <v>249.5</v>
       </c>
       <c r="M67" s="21">
         <v>2</v>
@@ -54915,36 +54915,36 @@
         <v>3</v>
       </c>
       <c r="E68" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.31770854521209096</v>
+      </c>
+      <c r="F68" s="21">
+        <f t="shared" ref="F68:F83" ca="1" si="17">F67+E68</f>
+        <v>0.65762327752776129</v>
+      </c>
+      <c r="G68" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>9.2970263999706149E-2</v>
-      </c>
-      <c r="F68" s="21">
-        <f t="shared" ref="F68:F83" ca="1" si="14">F67+E68</f>
-        <v>0.60731487519431604</v>
-      </c>
-      <c r="G68" s="21">
-        <f ca="1">ROUND(52*F68/F$84,0)</f>
         <v>5</v>
       </c>
       <c r="H68" s="28">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="11"/>
         <v>149</v>
       </c>
       <c r="I68" s="29">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="14"/>
         <v>246</v>
       </c>
       <c r="J68" s="21">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="15"/>
         <v>149</v>
       </c>
       <c r="K68" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>4.1231056256176606</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>15.297058540778355</v>
       </c>
       <c r="L68" s="21">
-        <f t="shared" ref="L68:L102" ca="1" si="15">(H68-H67)*(I67+I68)/2</f>
-        <v>986</v>
+        <f t="shared" ref="L68:L102" ca="1" si="18">(H68-H67)*(I67+I68)/2</f>
+        <v>3712.5</v>
       </c>
       <c r="M68" s="21">
         <v>3</v>
@@ -54968,36 +54968,36 @@
         <v>4</v>
       </c>
       <c r="E69" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>8.7178834055290366E-3</v>
+      </c>
+      <c r="F69" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>0.66634116093329032</v>
+      </c>
+      <c r="G69" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>0.26134569268160851</v>
-      </c>
-      <c r="F69" s="21">
+        <v>5</v>
+      </c>
+      <c r="H69" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>149</v>
+      </c>
+      <c r="I69" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>0.86866056787592449</v>
-      </c>
-      <c r="G69" s="21">
-        <f ca="1">ROUND(52*F69/F$84,0)</f>
-        <v>7</v>
-      </c>
-      <c r="H69" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>156</v>
-      </c>
-      <c r="I69" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J69" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>156</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>149</v>
       </c>
       <c r="K69" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>7.2801098892805181</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
       </c>
       <c r="L69" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1715</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
       </c>
       <c r="M69" s="21">
         <v>4</v>
@@ -55021,36 +55021,36 @@
         <v>5</v>
       </c>
       <c r="E70" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.39900171029512266</v>
+      </c>
+      <c r="F70" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.065342871228413</v>
+      </c>
+      <c r="G70" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>1.0490483380260041E-2</v>
-      </c>
-      <c r="F70" s="21">
+        <v>7</v>
+      </c>
+      <c r="H70" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>156</v>
+      </c>
+      <c r="I70" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>0.87915105125618453</v>
-      </c>
-      <c r="G70" s="21">
-        <f ca="1">ROUND(52*F70/F$84,0)</f>
-        <v>7</v>
-      </c>
-      <c r="H70" s="28">
-        <f t="shared" ca="1" si="8"/>
+        <v>244</v>
+      </c>
+      <c r="J70" s="21">
+        <f t="shared" ca="1" si="15"/>
         <v>156</v>
       </c>
-      <c r="I70" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>244</v>
-      </c>
-      <c r="J70" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>156</v>
-      </c>
       <c r="K70" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>7.2801098892805181</v>
       </c>
       <c r="L70" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>1715</v>
       </c>
       <c r="M70" s="21">
         <v>5</v>
@@ -55074,35 +55074,35 @@
         <v>6</v>
       </c>
       <c r="E71" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.41188185620114598</v>
+      </c>
+      <c r="F71" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.4772247274295589</v>
+      </c>
+      <c r="G71" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>0.29231639658885761</v>
-      </c>
-      <c r="F71" s="21">
+        <v>10</v>
+      </c>
+      <c r="H71" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>162</v>
+      </c>
+      <c r="I71" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>1.1714674478450422</v>
-      </c>
-      <c r="G71" s="21">
-        <f ca="1">ROUND(52*F71/F$84,0)</f>
-        <v>10</v>
-      </c>
-      <c r="H71" s="28">
-        <f t="shared" ca="1" si="8"/>
+        <v>242</v>
+      </c>
+      <c r="J71" s="21">
+        <f t="shared" ca="1" si="15"/>
         <v>162</v>
       </c>
-      <c r="I71" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>242</v>
-      </c>
-      <c r="J71" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>162</v>
-      </c>
       <c r="K71" s="21">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="16"/>
         <v>6.324555320336759</v>
       </c>
       <c r="L71" s="21">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="18"/>
         <v>1458</v>
       </c>
       <c r="M71" s="21">
@@ -55127,36 +55127,36 @@
         <v>7</v>
       </c>
       <c r="E72" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.38004803661249503</v>
+      </c>
+      <c r="F72" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>1.8572727640420539</v>
+      </c>
+      <c r="G72" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1259536642469346</v>
-      </c>
-      <c r="F72" s="21">
+        <v>13</v>
+      </c>
+      <c r="H72" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>168</v>
+      </c>
+      <c r="I72" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>1.2974211120919767</v>
-      </c>
-      <c r="G72" s="21">
-        <f ca="1">ROUND(52*F72/F$84,0)</f>
-        <v>11</v>
-      </c>
-      <c r="H72" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>165</v>
-      </c>
-      <c r="I72" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J72" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>165</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>168</v>
       </c>
       <c r="K72" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>3.1622776601683795</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>6.324555320336759</v>
       </c>
       <c r="L72" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>724.5</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>1446</v>
       </c>
       <c r="M72" s="21">
         <v>7</v>
@@ -55180,36 +55180,36 @@
         <v>8</v>
       </c>
       <c r="E73" s="21">
+        <f t="shared" ca="1" si="13"/>
+        <v>0.15914322474986359</v>
+      </c>
+      <c r="F73" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>2.0164159887919175</v>
+      </c>
+      <c r="G73" s="21">
         <f t="shared" ca="1" si="10"/>
-        <v>2.7687621942908858E-2</v>
-      </c>
-      <c r="F73" s="21">
+        <v>14</v>
+      </c>
+      <c r="H73" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>169</v>
+      </c>
+      <c r="I73" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>1.3251087340348855</v>
-      </c>
-      <c r="G73" s="21">
-        <f ca="1">ROUND(52*F73/F$84,0)</f>
-        <v>11</v>
-      </c>
-      <c r="H73" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>165</v>
-      </c>
-      <c r="I73" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J73" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>165</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>169</v>
       </c>
       <c r="K73" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>1.4142135623730951</v>
       </c>
       <c r="L73" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>239.5</v>
       </c>
       <c r="M73" s="21">
         <v>8</v>
@@ -55233,36 +55233,36 @@
         <v>9</v>
       </c>
       <c r="E74" s="21">
-        <f t="shared" ref="E74" ca="1" si="16">RAND()</f>
-        <v>5.5511154402607676E-2</v>
+        <f t="shared" ref="E74" ca="1" si="19">RAND()</f>
+        <v>0.92796135922819178</v>
       </c>
       <c r="F74" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>2.9443773480201094</v>
+      </c>
+      <c r="G74" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>21</v>
+      </c>
+      <c r="H74" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>182</v>
+      </c>
+      <c r="I74" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>1.3806198884374932</v>
-      </c>
-      <c r="G74" s="21">
-        <f ca="1">ROUND(52*F74/F$84,0)</f>
-        <v>12</v>
-      </c>
-      <c r="H74" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>167</v>
-      </c>
-      <c r="I74" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="J74" s="21">
-        <f t="shared" ca="1" si="12"/>
-        <v>167</v>
+        <f t="shared" ca="1" si="15"/>
+        <v>182</v>
       </c>
       <c r="K74" s="21">
-        <f t="shared" ca="1" si="13"/>
-        <v>2.2360679774997898</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>14.317821063276353</v>
       </c>
       <c r="L74" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>481</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>3068</v>
       </c>
       <c r="M74" s="21">
         <v>9</v>
@@ -55286,36 +55286,36 @@
         <v>10</v>
       </c>
       <c r="E75" s="21">
-        <f t="shared" ref="E75:E84" ca="1" si="17">RAND()</f>
-        <v>0.53390504963361918</v>
+        <f t="shared" ref="E75:E84" ca="1" si="20">RAND()</f>
+        <v>0.19775133585915439</v>
       </c>
       <c r="F75" s="21">
+        <f t="shared" ca="1" si="17"/>
+        <v>3.1421286838792639</v>
+      </c>
+      <c r="G75" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>22</v>
+      </c>
+      <c r="H75" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>183</v>
+      </c>
+      <c r="I75" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>1.9145249380711125</v>
-      </c>
-      <c r="G75" s="21">
-        <f ca="1">ROUND(52*F75/F$84,0)</f>
-        <v>16</v>
-      </c>
-      <c r="H75" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>172</v>
-      </c>
-      <c r="I75" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="J75" s="21">
-        <f t="shared" ref="J75:J83" ca="1" si="18">H75</f>
-        <v>172</v>
+        <f t="shared" ref="J75:J83" ca="1" si="21">H75</f>
+        <v>183</v>
       </c>
       <c r="K75" s="21">
         <f ca="1">SQRT((H74-H75)^2+(I74-I75)^2)</f>
-        <v>5.3851648071345037</v>
+        <v>1</v>
       </c>
       <c r="L75" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1195</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>233</v>
       </c>
       <c r="M75" s="21">
         <v>10</v>
@@ -55339,36 +55339,36 @@
         <v>11</v>
       </c>
       <c r="E76" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.58387881580048084</v>
+      </c>
+      <c r="F76" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.43346528034562137</v>
-      </c>
-      <c r="F76" s="21">
+        <v>3.7260074996797448</v>
+      </c>
+      <c r="G76" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>26</v>
+      </c>
+      <c r="H76" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>185</v>
+      </c>
+      <c r="I76" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>2.3479902184167338</v>
-      </c>
-      <c r="G76" s="21">
-        <f ca="1">ROUND(52*F76/F$84,0)</f>
-        <v>20</v>
-      </c>
-      <c r="H76" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="I76" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="J76" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>185</v>
+      </c>
+      <c r="K76" s="21">
+        <f t="shared" ref="K76:K83" ca="1" si="22">SQRT((H75-H76)^2+(I75-I76)^2)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="L76" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>180</v>
-      </c>
-      <c r="K76" s="21">
-        <f t="shared" ref="K76:K83" ca="1" si="19">SQRT((H75-H76)^2+(I75-I76)^2)</f>
-        <v>8.9442719099991592</v>
-      </c>
-      <c r="L76" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1888</v>
+        <v>464</v>
       </c>
       <c r="M76" s="21">
         <v>11</v>
@@ -55392,36 +55392,36 @@
         <v>12</v>
       </c>
       <c r="E77" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.54850527409787242</v>
+      </c>
+      <c r="F77" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.44955826820439015</v>
-      </c>
-      <c r="F77" s="21">
+        <v>4.2745127737776176</v>
+      </c>
+      <c r="G77" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="H77" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>190</v>
+      </c>
+      <c r="I77" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>2.7975484866211238</v>
-      </c>
-      <c r="G77" s="21">
-        <f ca="1">ROUND(52*F77/F$84,0)</f>
-        <v>24</v>
-      </c>
-      <c r="H77" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>184</v>
-      </c>
-      <c r="I77" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J77" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>190</v>
+      </c>
+      <c r="K77" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="L77" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>184</v>
-      </c>
-      <c r="K77" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="L77" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>932</v>
+        <v>1147.5</v>
       </c>
       <c r="M77" s="21">
         <v>12</v>
@@ -55445,36 +55445,36 @@
         <v>13</v>
       </c>
       <c r="E78" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.68907483208636111</v>
+      </c>
+      <c r="F78" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.99690687087002194</v>
-      </c>
-      <c r="F78" s="21">
+        <v>4.963587605863979</v>
+      </c>
+      <c r="G78" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>35</v>
+      </c>
+      <c r="H78" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>194</v>
+      </c>
+      <c r="I78" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>3.7944553574911457</v>
-      </c>
-      <c r="G78" s="21">
-        <f ca="1">ROUND(52*F78/F$84,0)</f>
-        <v>32</v>
-      </c>
-      <c r="H78" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>191</v>
-      </c>
-      <c r="I78" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J78" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>194</v>
+      </c>
+      <c r="K78" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="L78" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>191</v>
-      </c>
-      <c r="K78" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>8.6023252670426267</v>
-      </c>
-      <c r="L78" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1606.5</v>
+        <v>906</v>
       </c>
       <c r="M78" s="21">
         <v>13</v>
@@ -55498,36 +55498,36 @@
         <v>14</v>
       </c>
       <c r="E79" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.72062165602272366</v>
+      </c>
+      <c r="F79" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>3.5460398381747638E-2</v>
-      </c>
-      <c r="F79" s="21">
+        <v>5.6842092618867026</v>
+      </c>
+      <c r="G79" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="H79" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>200</v>
+      </c>
+      <c r="I79" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8299157558728933</v>
-      </c>
-      <c r="G79" s="21">
-        <f ca="1">ROUND(52*F79/F$84,0)</f>
-        <v>32</v>
-      </c>
-      <c r="H79" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>191</v>
-      </c>
-      <c r="I79" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J79" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>200</v>
+      </c>
+      <c r="K79" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>7.2111025509279782</v>
+      </c>
+      <c r="L79" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>191</v>
-      </c>
-      <c r="K79" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L79" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1338</v>
       </c>
       <c r="M79" s="21">
         <v>14</v>
@@ -55551,36 +55551,36 @@
         <v>15</v>
       </c>
       <c r="E80" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.91272187972540775</v>
+      </c>
+      <c r="F80" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>5.0597989464220561E-2</v>
-      </c>
-      <c r="F80" s="21">
+        <v>6.5969311416121101</v>
+      </c>
+      <c r="G80" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>46</v>
+      </c>
+      <c r="H80" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>204</v>
+      </c>
+      <c r="I80" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>3.8805137453371139</v>
-      </c>
-      <c r="G80" s="21">
-        <f ca="1">ROUND(52*F80/F$84,0)</f>
-        <v>33</v>
-      </c>
-      <c r="H80" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>193</v>
-      </c>
-      <c r="I80" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="J80" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>204</v>
+      </c>
+      <c r="K80" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="L80" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>193</v>
-      </c>
-      <c r="K80" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>2.2360679774997898</v>
-      </c>
-      <c r="L80" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>453</v>
+        <v>878</v>
       </c>
       <c r="M80" s="21">
         <v>15</v>
@@ -55604,36 +55604,36 @@
         <v>16</v>
       </c>
       <c r="E81" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>1.6524689137193516E-2</v>
+      </c>
+      <c r="F81" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.72516100622627189</v>
-      </c>
-      <c r="F81" s="21">
+        <v>6.6134558307493041</v>
+      </c>
+      <c r="G81" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>46</v>
+      </c>
+      <c r="H81" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>204</v>
+      </c>
+      <c r="I81" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>4.6056747515633862</v>
-      </c>
-      <c r="G81" s="21">
-        <f ca="1">ROUND(52*F81/F$84,0)</f>
-        <v>39</v>
-      </c>
-      <c r="H81" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>198</v>
-      </c>
-      <c r="I81" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="J81" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>204</v>
+      </c>
+      <c r="K81" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="L81" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>198</v>
-      </c>
-      <c r="K81" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>6.4031242374328485</v>
-      </c>
-      <c r="L81" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1120</v>
+        <v>0</v>
       </c>
       <c r="M81" s="21">
         <v>16</v>
@@ -55657,36 +55657,36 @@
         <v>17</v>
       </c>
       <c r="E82" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>9.2257066587688952E-2</v>
+      </c>
+      <c r="F82" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.61068454488600032</v>
-      </c>
-      <c r="F82" s="21">
+        <v>6.7057128973369933</v>
+      </c>
+      <c r="G82" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>47</v>
+      </c>
+      <c r="H82" s="28">
+        <f t="shared" ca="1" si="11"/>
+        <v>204</v>
+      </c>
+      <c r="I82" s="29">
         <f t="shared" ca="1" si="14"/>
-        <v>5.2163592964493866</v>
-      </c>
-      <c r="G82" s="21">
-        <f ca="1">ROUND(52*F82/F$84,0)</f>
-        <v>44</v>
-      </c>
-      <c r="H82" s="28">
-        <f t="shared" ca="1" si="8"/>
-        <v>203</v>
-      </c>
-      <c r="I82" s="29">
-        <f t="shared" ca="1" si="11"/>
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J82" s="21">
+        <f t="shared" ca="1" si="21"/>
+        <v>204</v>
+      </c>
+      <c r="K82" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="L82" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>203</v>
-      </c>
-      <c r="K82" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>5.8309518948453007</v>
-      </c>
-      <c r="L82" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1102.5</v>
+        <v>0</v>
       </c>
       <c r="M82" s="21">
         <v>17</v>
@@ -55710,36 +55710,36 @@
         <v>18</v>
       </c>
       <c r="E83" s="21">
+        <f t="shared" ca="1" si="20"/>
+        <v>0.38657196065515531</v>
+      </c>
+      <c r="F83" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0.66041126851467025</v>
-      </c>
-      <c r="F83" s="21">
+        <v>7.0922848579921487</v>
+      </c>
+      <c r="G83" s="21">
+        <f t="shared" ca="1" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="H83" s="30">
+        <f t="shared" ca="1" si="11"/>
+        <v>209</v>
+      </c>
+      <c r="I83" s="31">
         <f t="shared" ca="1" si="14"/>
-        <v>5.8767705649640565</v>
-      </c>
-      <c r="G83" s="21">
-        <f ca="1">ROUND(52*F83/F$84,0)</f>
-        <v>50</v>
-      </c>
-      <c r="H83" s="30">
-        <f t="shared" ca="1" si="8"/>
+        <v>213</v>
+      </c>
+      <c r="J83" s="21">
+        <f t="shared" ca="1" si="21"/>
         <v>209</v>
       </c>
-      <c r="I83" s="31">
-        <f t="shared" ca="1" si="11"/>
-        <v>213</v>
-      </c>
-      <c r="J83" s="21">
+      <c r="K83" s="21">
+        <f t="shared" ca="1" si="22"/>
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="L83" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>209</v>
-      </c>
-      <c r="K83" s="21">
-        <f t="shared" ca="1" si="19"/>
-        <v>8.4852813742385695</v>
-      </c>
-      <c r="L83" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1296</v>
+        <v>1075</v>
       </c>
       <c r="M83" s="21">
         <v>18</v>
@@ -55763,15 +55763,15 @@
         <v>19</v>
       </c>
       <c r="E84" s="21">
-        <f t="shared" ca="1" si="17"/>
-        <v>0.25788026624458871</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>0.34339365198580174</v>
       </c>
       <c r="F84" s="21">
-        <f t="shared" ref="F84" ca="1" si="20">F83+E84</f>
-        <v>6.1346508312086456</v>
+        <f t="shared" ref="F84" ca="1" si="23">F83+E84</f>
+        <v>7.4356785099779508</v>
       </c>
       <c r="G84" s="21">
-        <f ca="1">ROUND(52*F84/F$84,0)</f>
+        <f t="shared" ca="1" si="10"/>
         <v>52</v>
       </c>
       <c r="H84" s="32">
@@ -55783,15 +55783,15 @@
         <v>209</v>
       </c>
       <c r="J84" s="21">
-        <f t="shared" ref="J84" ca="1" si="21">H84</f>
+        <f t="shared" ref="J84" ca="1" si="24">H84</f>
         <v>213</v>
       </c>
       <c r="K84" s="21">
-        <f t="shared" ref="K84" ca="1" si="22">SQRT((H83-H84)^2+(I83-I84)^2)</f>
+        <f t="shared" ref="K84" ca="1" si="25">SQRT((H83-H84)^2+(I83-I84)^2)</f>
         <v>5.6568542494923806</v>
       </c>
       <c r="L84" s="21">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="18"/>
         <v>844</v>
       </c>
       <c r="M84" s="21">
@@ -55817,23 +55817,23 @@
       </c>
       <c r="H85" s="34">
         <f ca="1">I82</f>
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I85" s="35">
         <f ca="1">H82</f>
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J85" s="21">
-        <f t="shared" ref="J85:J102" ca="1" si="23">H85</f>
-        <v>219</v>
+        <f t="shared" ref="J85:J102" ca="1" si="26">H85</f>
+        <v>217</v>
       </c>
       <c r="K85" s="21">
-        <f t="shared" ref="K85:K102" ca="1" si="24">SQRT((H84-H85)^2+(I84-I85)^2)</f>
-        <v>8.4852813742385695</v>
+        <f t="shared" ref="K85:K102" ca="1" si="27">SQRT((H84-H85)^2+(I84-I85)^2)</f>
+        <v>6.4031242374328485</v>
       </c>
       <c r="L85" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>1236</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>826</v>
       </c>
       <c r="M85" s="21">
         <v>20</v>
@@ -55858,23 +55858,23 @@
       </c>
       <c r="H86" s="34">
         <f ca="1">I81</f>
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I86" s="35">
         <f ca="1">H81</f>
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="J86" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>222</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>218</v>
       </c>
       <c r="K86" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>5.8309518948453007</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>1</v>
       </c>
       <c r="L86" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>601.5</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>204</v>
       </c>
       <c r="M86" s="21">
         <v>21</v>
@@ -55899,23 +55899,23 @@
       </c>
       <c r="H87" s="34">
         <f ca="1">I80</f>
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="I87" s="35">
         <f ca="1">H80</f>
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="J87" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>226</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>218</v>
       </c>
       <c r="K87" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>6.4031242374328485</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>0</v>
       </c>
       <c r="L87" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>782</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
       </c>
       <c r="M87" s="21">
         <v>22</v>
@@ -55940,23 +55940,23 @@
       </c>
       <c r="H88" s="34">
         <f ca="1">I79</f>
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I88" s="35">
         <f ca="1">H79</f>
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="J88" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>227</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>221</v>
       </c>
       <c r="K88" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>2.2360679774997898</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>5</v>
       </c>
       <c r="L88" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>192</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>606</v>
       </c>
       <c r="M88" s="21">
         <v>23</v>
@@ -55981,23 +55981,23 @@
       </c>
       <c r="H89" s="34">
         <f ca="1">I78</f>
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I89" s="35">
         <f ca="1">H78</f>
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="J89" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>227</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>225</v>
       </c>
       <c r="K89" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>7.2111025509279782</v>
       </c>
       <c r="L89" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>788</v>
       </c>
       <c r="M89" s="21">
         <v>24</v>
@@ -56022,23 +56022,23 @@
       </c>
       <c r="H90" s="34">
         <f ca="1">I77</f>
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I90" s="35">
         <f ca="1">H77</f>
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="J90" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>232</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>228</v>
       </c>
       <c r="K90" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>8.6023252670426267</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>5</v>
       </c>
       <c r="L90" s="21">
         <f ca="1">(H90-H89)*(I89+I90)/2</f>
-        <v>937.5</v>
+        <v>576</v>
       </c>
       <c r="M90" s="21">
         <v>25</v>
@@ -56063,23 +56063,23 @@
       </c>
       <c r="H91" s="34">
         <f ca="1">I76</f>
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I91" s="35">
         <f ca="1">H76</f>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="J91" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>234</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>231</v>
       </c>
       <c r="K91" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>4.4721359549995796</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>5.8309518948453007</v>
       </c>
       <c r="L91" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>364</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>562.5</v>
       </c>
       <c r="M91" s="21">
         <v>26</v>
@@ -56104,23 +56104,23 @@
       </c>
       <c r="H92" s="34">
         <f ca="1">I75</f>
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I92" s="35">
         <f ca="1">H75</f>
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="J92" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>238</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>233</v>
       </c>
       <c r="K92" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>8.9442719099991592</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>2.8284271247461903</v>
       </c>
       <c r="L92" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>704</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>368</v>
       </c>
       <c r="M92" s="21">
         <v>27</v>
@@ -56138,23 +56138,23 @@
       </c>
       <c r="H93" s="34">
         <f ca="1">I74</f>
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I93" s="35">
         <f ca="1">H74</f>
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J93" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>240</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>233</v>
       </c>
       <c r="K93" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>5.3851648071345037</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>1</v>
       </c>
       <c r="L93" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>339</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
       </c>
       <c r="M93" s="21">
         <v>28</v>
@@ -56172,23 +56172,23 @@
       </c>
       <c r="H94" s="34">
         <f ca="1">I73</f>
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I94" s="35">
         <f ca="1">H73</f>
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J94" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>241</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>239</v>
       </c>
       <c r="K94" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>2.2360679774997898</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>14.317821063276353</v>
       </c>
       <c r="L94" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>166</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>1053</v>
       </c>
       <c r="M94" s="21">
         <v>29</v>
@@ -56206,23 +56206,23 @@
       </c>
       <c r="H95" s="34">
         <f ca="1">I72</f>
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I95" s="35">
         <f ca="1">H72</f>
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J95" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>241</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>240</v>
       </c>
       <c r="K95" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>1.4142135623730951</v>
       </c>
       <c r="L95" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>168.5</v>
       </c>
       <c r="M95" s="21">
         <v>30</v>
@@ -56247,16 +56247,16 @@
         <v>162</v>
       </c>
       <c r="J96" s="21">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="26"/>
         <v>242</v>
       </c>
       <c r="K96" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>3.1622776601683795</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>6.324555320336759</v>
       </c>
       <c r="L96" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>163.5</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>330</v>
       </c>
       <c r="M96" s="21">
         <v>31</v>
@@ -56281,15 +56281,15 @@
         <v>156</v>
       </c>
       <c r="J97" s="21">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="26"/>
         <v>244</v>
       </c>
       <c r="K97" s="21">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="27"/>
         <v>6.324555320336759</v>
       </c>
       <c r="L97" s="21">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="18"/>
         <v>318</v>
       </c>
       <c r="M97" s="21">
@@ -56308,23 +56308,23 @@
       </c>
       <c r="H98" s="34">
         <f ca="1">I69</f>
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I98" s="35">
         <f ca="1">H69</f>
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J98" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>244</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>246</v>
       </c>
       <c r="K98" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>7.2801098892805181</v>
       </c>
       <c r="L98" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>305</v>
       </c>
       <c r="M98" s="21">
         <v>33</v>
@@ -56349,16 +56349,16 @@
         <v>149</v>
       </c>
       <c r="J99" s="21">
-        <f t="shared" ca="1" si="23"/>
+        <f t="shared" ca="1" si="26"/>
         <v>246</v>
       </c>
       <c r="K99" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>7.2801098892805181</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>0</v>
       </c>
       <c r="L99" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>305</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
       </c>
       <c r="M99" s="21">
         <v>34</v>
@@ -56376,23 +56376,23 @@
       </c>
       <c r="H100" s="34">
         <f ca="1">I67</f>
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I100" s="35">
         <f ca="1">H67</f>
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="J100" s="21">
-        <f t="shared" ca="1" si="23"/>
-        <v>247</v>
+        <f t="shared" ca="1" si="26"/>
+        <v>249</v>
       </c>
       <c r="K100" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>4.1231056256176606</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>15.297058540778355</v>
       </c>
       <c r="L100" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>147</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>424.5</v>
       </c>
       <c r="M100" s="21">
         <v>35</v>
@@ -56414,19 +56414,19 @@
       </c>
       <c r="I101" s="35">
         <f ca="1">H66</f>
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="J101" s="21">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>250</v>
       </c>
       <c r="K101" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>5.8309518948453007</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>1.4142135623730951</v>
       </c>
       <c r="L101" s="21">
-        <f t="shared" ca="1" si="15"/>
-        <v>427.5</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>133.5</v>
       </c>
       <c r="M101" s="21">
         <v>36</v>
@@ -56451,15 +56451,15 @@
         <v>0</v>
       </c>
       <c r="J102" s="21">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>250</v>
       </c>
       <c r="K102" s="21">
-        <f t="shared" ca="1" si="24"/>
-        <v>140</v>
+        <f t="shared" ca="1" si="27"/>
+        <v>133</v>
       </c>
       <c r="L102" s="21">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="18"/>
         <v>0</v>
       </c>
       <c r="M102">
@@ -56475,15 +56475,15 @@
     <row r="104" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K104" s="21">
         <f ca="1">SUM(K66:K102)</f>
-        <v>444.28963783137402</v>
+        <v>444.94912038290698</v>
       </c>
       <c r="L104" s="21">
         <f ca="1">SUM(L66:L102)</f>
-        <v>58727</v>
+        <v>58687</v>
       </c>
       <c r="M104" s="4">
         <f ca="1">L104/K104</f>
-        <v>132.18179088455196</v>
+        <v>131.89597936387898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>